<commit_message>
DATABASE: fixed wrong file sizes, modified with new file sizes, added entries for J - Q
</commit_message>
<xml_diff>
--- a/resources/database/data/anime/db_anime - staging data.xlsx
+++ b/resources/database/data/anime/db_anime - staging data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3000" windowWidth="24000" windowHeight="9495" tabRatio="813" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="3600" windowWidth="24000" windowHeight="9495" tabRatio="813"/>
   </bookViews>
   <sheets>
     <sheet name="&gt;&gt;Final" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3780" uniqueCount="664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3789" uniqueCount="668">
   <si>
     <t>Summer</t>
   </si>
@@ -2026,6 +2026,18 @@
   </si>
   <si>
     <t>Suzumiya Haruhi no Shoushitsu (Movie), Suzumiya Haruhi-chan no Yuuutsu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Naruto Shippuuden</t>
+  </si>
+  <si>
+    <t>One Piece</t>
+  </si>
+  <si>
+    <t>NULL</t>
   </si>
 </sst>
 </file>
@@ -2493,16 +2505,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA243"/>
+  <dimension ref="A1:AA245"/>
   <sheetViews>
-    <sheetView topLeftCell="A229" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A230" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="J1" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="D249" sqref="D249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.5703125" customWidth="1"/>
+    <col min="4" max="4" width="43.7109375" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="23.7109375" customWidth="1"/>
@@ -4494,7 +4508,7 @@
         <v>0</v>
       </c>
       <c r="H30">
-        <v>6908773272</v>
+        <v>2513965439</v>
       </c>
       <c r="I30">
         <v>1</v>
@@ -5284,7 +5298,7 @@
         <v>1</v>
       </c>
       <c r="H42">
-        <v>7320844419</v>
+        <v>5703465871</v>
       </c>
       <c r="I42">
         <v>2</v>
@@ -5350,7 +5364,7 @@
         <v>0</v>
       </c>
       <c r="H43">
-        <v>7910330633</v>
+        <v>2802892114</v>
       </c>
       <c r="I43">
         <v>1</v>
@@ -6014,7 +6028,7 @@
         <v>2</v>
       </c>
       <c r="H53">
-        <v>10227323699</v>
+        <v>3761255977</v>
       </c>
       <c r="I53">
         <v>2</v>
@@ -6085,7 +6099,7 @@
         <v>0</v>
       </c>
       <c r="H54">
-        <v>3461703367</v>
+        <v>1445683409</v>
       </c>
       <c r="I54">
         <v>1</v>
@@ -7851,7 +7865,7 @@
         <v>0</v>
       </c>
       <c r="H80">
-        <v>8744652783</v>
+        <v>3434857496</v>
       </c>
       <c r="I80">
         <v>1</v>
@@ -8795,7 +8809,7 @@
         <v>0</v>
       </c>
       <c r="H94">
-        <v>16394832712</v>
+        <v>6357494190</v>
       </c>
       <c r="I94">
         <v>1</v>
@@ -8866,7 +8880,7 @@
         <v>0</v>
       </c>
       <c r="H95">
-        <v>7805298612</v>
+        <v>3310112137</v>
       </c>
       <c r="I95">
         <v>1</v>
@@ -18395,6 +18409,106 @@
         <v>0</v>
       </c>
       <c r="AA243">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <v>242</v>
+      </c>
+      <c r="B244">
+        <v>1</v>
+      </c>
+      <c r="C244" t="s">
+        <v>7</v>
+      </c>
+      <c r="D244" t="s">
+        <v>665</v>
+      </c>
+      <c r="E244">
+        <v>96</v>
+      </c>
+      <c r="F244">
+        <v>0</v>
+      </c>
+      <c r="G244">
+        <v>0</v>
+      </c>
+      <c r="H244">
+        <v>4831397928</v>
+      </c>
+      <c r="I244">
+        <v>1</v>
+      </c>
+      <c r="J244" t="s">
+        <v>665</v>
+      </c>
+      <c r="N244" s="9" t="s">
+        <v>667</v>
+      </c>
+      <c r="W244">
+        <v>1</v>
+      </c>
+      <c r="X244">
+        <v>0</v>
+      </c>
+      <c r="Y244">
+        <v>0</v>
+      </c>
+      <c r="Z244">
+        <v>0</v>
+      </c>
+      <c r="AA244">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <v>243</v>
+      </c>
+      <c r="B245">
+        <v>1</v>
+      </c>
+      <c r="C245" t="s">
+        <v>5</v>
+      </c>
+      <c r="D245" t="s">
+        <v>666</v>
+      </c>
+      <c r="E245">
+        <v>798</v>
+      </c>
+      <c r="F245">
+        <v>0</v>
+      </c>
+      <c r="G245">
+        <v>0</v>
+      </c>
+      <c r="H245">
+        <v>174992242032</v>
+      </c>
+      <c r="I245">
+        <v>1</v>
+      </c>
+      <c r="J245" t="s">
+        <v>666</v>
+      </c>
+      <c r="N245" s="9" t="s">
+        <v>667</v>
+      </c>
+      <c r="W245">
+        <v>1</v>
+      </c>
+      <c r="X245">
+        <v>0</v>
+      </c>
+      <c r="Y245">
+        <v>0</v>
+      </c>
+      <c r="Z245">
+        <v>0</v>
+      </c>
+      <c r="AA245">
         <v>0</v>
       </c>
     </row>
@@ -24203,7 +24317,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -29037,10 +29151,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B121"/>
+  <dimension ref="A1:J121"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29048,972 +29162,1459 @@
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>2325657902</v>
       </c>
       <c r="B1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J1">
+        <f>A1/1024/1024/1024</f>
+        <v>2.1659377049654722</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3849568040</v>
       </c>
       <c r="B2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <f t="shared" ref="J2:J65" si="0">A2/1024/1024/1024</f>
+        <v>3.5851896181702614</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4289938905</v>
       </c>
       <c r="B3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <f t="shared" si="0"/>
+        <v>3.9953169459477067</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>8450070047</v>
       </c>
       <c r="B4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>7.8697409918531775</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>12780605656</v>
       </c>
       <c r="B5" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>11.902866564691067</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>9697671057</v>
       </c>
       <c r="B6" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>9.0316599765792489</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4616293384</v>
       </c>
       <c r="B7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>4.2992582395672798</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4261331962</v>
       </c>
       <c r="B8" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>3.9686746541410685</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4442742278</v>
       </c>
       <c r="B9" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>4.137626176699996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5788975826</v>
       </c>
       <c r="B10" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>5.3914038706570864</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9027296173</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>8.4073247136548162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5018873005</v>
       </c>
       <c r="B12" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>4.6741897286847234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>532778690</v>
       </c>
       <c r="B13" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>664</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>0.4961888212710619</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>84523909</v>
       </c>
       <c r="B14" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>7.8719024546444416E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1206029695</v>
       </c>
       <c r="B15" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>1.1232026806101203</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>10435858309</v>
       </c>
       <c r="B16" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>9.7191504286602139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>12416450410</v>
       </c>
       <c r="B17" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>11.563720563426614</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>7241097661</v>
       </c>
       <c r="B18" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>6.7437977166846395</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>671219731</v>
       </c>
       <c r="B19" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>0.62512208800762892</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>8087379115</v>
       </c>
       <c r="B20" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>7.5319587392732501</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>7320844419</v>
       </c>
       <c r="B21" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>6.818067672662437</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>7910330633</v>
       </c>
       <c r="B22" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>7.3670694911852479</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>8104821238</v>
       </c>
       <c r="B23" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>7.54820298217237</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>8174459847</v>
       </c>
       <c r="B24" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>7.6130589907988906</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>7783211114</v>
       </c>
       <c r="B25" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>7.2486802134662867</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>4075620960</v>
       </c>
       <c r="B26" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>3.7957178056240082</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>5486616265</v>
       </c>
       <c r="B27" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J27">
+        <f t="shared" si="0"/>
+        <v>5.1098095858469605</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1390427359</v>
       </c>
       <c r="B28" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J28">
+        <f t="shared" si="0"/>
+        <v>1.2949363877996802</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>239307157</v>
       </c>
       <c r="B29" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J29">
+        <f t="shared" si="0"/>
+        <v>0.22287215758115053</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>19552073210</v>
       </c>
       <c r="B30" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J30">
+        <f t="shared" si="0"/>
+        <v>18.209287161007524</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>3884499924</v>
       </c>
       <c r="B31" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J31">
+        <f t="shared" si="0"/>
+        <v>3.6177224703133106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>5053981140</v>
       </c>
       <c r="B32" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J32">
+        <f t="shared" si="0"/>
+        <v>4.7068867273628712</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>3160175258</v>
       </c>
       <c r="B33" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J33">
+        <f t="shared" si="0"/>
+        <v>2.9431425575166941</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>7894452816</v>
       </c>
       <c r="B34" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J34">
+        <f t="shared" si="0"/>
+        <v>7.3522821217775345</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3099970850</v>
       </c>
       <c r="B35" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J35">
+        <f t="shared" si="0"/>
+        <v>2.8870728332549334</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>5296543763</v>
       </c>
       <c r="B36" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J36">
+        <f t="shared" si="0"/>
+        <v>4.9327907739207149</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>10227323699</v>
       </c>
       <c r="B37" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J37">
+        <f t="shared" si="0"/>
+        <v>9.5249374387785792</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>3461703367</v>
       </c>
       <c r="B38" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J38">
+        <f t="shared" si="0"/>
+        <v>3.2239624923095107</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>6097715390</v>
       </c>
       <c r="B39" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J39">
+        <f t="shared" si="0"/>
+        <v>5.6789399962872267</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>940589673</v>
       </c>
       <c r="B40" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J40">
+        <f t="shared" si="0"/>
+        <v>0.87599239591509104</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>5365959816</v>
       </c>
       <c r="B41" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J41">
+        <f t="shared" si="0"/>
+        <v>4.9974395111203194</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>8131289060</v>
       </c>
       <c r="B42" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J42">
+        <f t="shared" si="0"/>
+        <v>7.5728530623018742</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>4671496823</v>
       </c>
       <c r="B43" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J43">
+        <f t="shared" si="0"/>
+        <v>4.3506704485043883</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1140794207</v>
       </c>
       <c r="B44" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J44">
+        <f t="shared" si="0"/>
+        <v>1.0624473979696631</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>719854024</v>
       </c>
       <c r="B45" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J45">
+        <f t="shared" si="0"/>
+        <v>0.67041630297899246</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>6328334291</v>
       </c>
       <c r="B46" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J46">
+        <f t="shared" si="0"/>
+        <v>5.8937205849215388</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>7391556278</v>
       </c>
       <c r="B47" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J47">
+        <f t="shared" si="0"/>
+        <v>6.8839232232421637</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>8630813790</v>
       </c>
       <c r="B48" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J48">
+        <f t="shared" si="0"/>
+        <v>8.0380717199295759</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>3578168937</v>
       </c>
       <c r="B49" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J49">
+        <f t="shared" si="0"/>
+        <v>3.3324295068159699</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>5169851434</v>
       </c>
       <c r="B50" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J50">
+        <f t="shared" si="0"/>
+        <v>4.8147993478924036</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1315220278</v>
       </c>
       <c r="B51" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J51">
+        <f t="shared" si="0"/>
+        <v>1.2248943354934454</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1521655969</v>
       </c>
       <c r="B52" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J52">
+        <f t="shared" si="0"/>
+        <v>1.4171525547280908</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>9553342424</v>
       </c>
       <c r="B53" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J53">
+        <f t="shared" si="0"/>
+        <v>8.8972434625029564</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>9980890419</v>
       </c>
       <c r="B54" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J54">
+        <f t="shared" si="0"/>
+        <v>9.2954285619780421</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>4688852004</v>
       </c>
       <c r="B55" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J55">
+        <f t="shared" si="0"/>
+        <v>4.366833720356226</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>3800601454</v>
       </c>
       <c r="B56" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J56">
+        <f t="shared" si="0"/>
+        <v>3.5395859312266111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>650623681</v>
       </c>
       <c r="B57" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J57">
+        <f t="shared" si="0"/>
+        <v>0.60594052169471979</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>3782861568</v>
       </c>
       <c r="B58" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J58">
+        <f t="shared" si="0"/>
+        <v>3.5230643749237061</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>7511129124</v>
       </c>
       <c r="B59" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J59">
+        <f t="shared" si="0"/>
+        <v>6.9952841140329838</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>4883188053</v>
       </c>
       <c r="B60" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J60">
+        <f t="shared" si="0"/>
+        <v>4.5478232698515058</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>4583944069</v>
       </c>
       <c r="B61" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J61">
+        <f t="shared" si="0"/>
+        <v>4.2691305922344327</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>4485955223</v>
       </c>
       <c r="B62" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J62">
+        <f t="shared" si="0"/>
+        <v>4.1778713678941131</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>837972378</v>
       </c>
       <c r="B63" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J63">
+        <f t="shared" si="0"/>
+        <v>0.78042259253561497</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>4084622283</v>
       </c>
       <c r="B64" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J64">
+        <f t="shared" si="0"/>
+        <v>3.8041009409353137</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>4059872111</v>
       </c>
       <c r="B65" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J65">
+        <f t="shared" si="0"/>
+        <v>3.7810505470260978</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>4048571600</v>
       </c>
       <c r="B66" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J66">
+        <f t="shared" ref="J66:J121" si="1">A66/1024/1024/1024</f>
+        <v>3.7705261260271072</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>3166102301</v>
       </c>
       <c r="B67" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J67">
+        <f t="shared" si="1"/>
+        <v>2.9486625464633107</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>3583632982</v>
       </c>
       <c r="B68" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J68">
+        <f t="shared" si="1"/>
+        <v>3.3375182952731848</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>3175813204</v>
       </c>
       <c r="B69" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J69">
+        <f t="shared" si="1"/>
+        <v>2.9577065296471119</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>8893366380</v>
       </c>
       <c r="B70" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J70">
+        <f t="shared" si="1"/>
+        <v>8.2825928740203381</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>32872296460</v>
       </c>
       <c r="B71" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J71">
+        <f t="shared" si="1"/>
+        <v>30.61471177265048</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>21496101847</v>
       </c>
       <c r="B72" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J72">
+        <f t="shared" si="1"/>
+        <v>20.019804916344583</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>5810517001</v>
       </c>
       <c r="B73" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J73">
+        <f t="shared" si="1"/>
+        <v>5.411465653218329</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>8081890097</v>
       </c>
       <c r="B74" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J74">
+        <f t="shared" si="1"/>
+        <v>7.5268466928973794</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>13564258520</v>
       </c>
       <c r="B75" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J75">
+        <f t="shared" si="1"/>
+        <v>12.63270016759634</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>11465605176</v>
       </c>
       <c r="B76" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J76">
+        <f t="shared" si="1"/>
+        <v>10.678176932036877</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>8744652783</v>
       </c>
       <c r="B77" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J77">
+        <f t="shared" si="1"/>
+        <v>8.1440925439819694</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>1489281199</v>
       </c>
       <c r="B78" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J78">
+        <f t="shared" si="1"/>
+        <v>1.3870012005791068</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>646679926</v>
       </c>
       <c r="B79" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J79">
+        <f t="shared" si="1"/>
+        <v>0.60226761363446712</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>12100644006</v>
       </c>
       <c r="B80" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J80">
+        <f t="shared" si="1"/>
+        <v>11.269602930173278</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>14553369461</v>
       </c>
       <c r="B81" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J81">
+        <f t="shared" si="1"/>
+        <v>13.553881515748799</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>4402585407</v>
       </c>
       <c r="B82" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J82">
+        <f t="shared" si="1"/>
+        <v>4.1002271762117743</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>9848869212</v>
       </c>
       <c r="B83" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J83">
+        <f t="shared" si="1"/>
+        <v>9.1724742315709591</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>15850016027</v>
       </c>
       <c r="B84" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J84">
+        <f t="shared" si="1"/>
+        <v>14.761477733962238</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>9392851902</v>
       </c>
       <c r="B85" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J85">
+        <f t="shared" si="1"/>
+        <v>8.7477750163525343</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>33467813443</v>
       </c>
       <c r="B86" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J86">
+        <f t="shared" si="1"/>
+        <v>31.169330182485282</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>4389910869</v>
       </c>
       <c r="B87" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J87">
+        <f t="shared" si="1"/>
+        <v>4.0884230928495526</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>5762428879</v>
       </c>
       <c r="B88" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J88">
+        <f t="shared" si="1"/>
+        <v>5.3666800996288657</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>4282390294</v>
       </c>
       <c r="B89" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J89">
+        <f t="shared" si="1"/>
+        <v>3.988286754116416</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2852012355</v>
       </c>
       <c r="B90" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J90">
+        <f t="shared" si="1"/>
+        <v>2.6561434892937541</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>5235314867</v>
       </c>
       <c r="B91" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J91">
+        <f t="shared" si="1"/>
+        <v>4.8757669208571315</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>4864328790</v>
       </c>
       <c r="B92" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J92">
+        <f t="shared" si="1"/>
+        <v>4.5302592124789953</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>6892821396</v>
       </c>
       <c r="B93" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J93">
+        <f t="shared" si="1"/>
+        <v>6.4194401688873768</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>5172115229</v>
       </c>
       <c r="B94" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J94">
+        <f t="shared" si="1"/>
+        <v>4.8169076712802052</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>5115002689</v>
       </c>
       <c r="B95" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J95">
+        <f t="shared" si="1"/>
+        <v>4.7637174734845757</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>13289369158</v>
       </c>
       <c r="B96" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J96">
+        <f t="shared" si="1"/>
+        <v>12.376689499244094</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2423318739</v>
       </c>
       <c r="B97" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J97">
+        <f t="shared" si="1"/>
+        <v>2.2568914471194148</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>887105350</v>
       </c>
       <c r="B98" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J98">
+        <f t="shared" si="1"/>
+        <v>0.82618123851716518</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>675892106</v>
       </c>
       <c r="B99" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J99">
+        <f t="shared" si="1"/>
+        <v>0.62947357632219791</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2600968426</v>
       </c>
       <c r="B100" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J100">
+        <f t="shared" si="1"/>
+        <v>2.4223406109958887</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>965276887</v>
       </c>
       <c r="B101" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J101">
+        <f t="shared" si="1"/>
+        <v>0.89898415561765432</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>1895067442</v>
       </c>
       <c r="B102" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J102">
+        <f t="shared" si="1"/>
+        <v>1.764919089153409</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>4818218700</v>
       </c>
       <c r="B103" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J103">
+        <f t="shared" si="1"/>
+        <v>4.4873158447444439</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>16394832712</v>
       </c>
       <c r="B104" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J104">
+        <f t="shared" si="1"/>
+        <v>15.268877811729908</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>13273149341</v>
       </c>
       <c r="B105" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J105">
+        <f t="shared" si="1"/>
+        <v>12.361583617515862</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>7805298612</v>
       </c>
       <c r="B106" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J106">
+        <f t="shared" si="1"/>
+        <v>7.2692507989704609</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>12915404039</v>
       </c>
       <c r="B107" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J107">
+        <f t="shared" si="1"/>
+        <v>12.02840734180063</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>6604812827</v>
       </c>
       <c r="B108" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J108">
+        <f t="shared" si="1"/>
+        <v>6.1512112868949771</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>1030103823</v>
       </c>
       <c r="B109" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J109">
+        <f t="shared" si="1"/>
+        <v>0.95935894455760717</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>669279215</v>
       </c>
       <c r="B110" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J110">
+        <f t="shared" si="1"/>
+        <v>0.62331484165042639</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>9060174840</v>
       </c>
       <c r="B111" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J111">
+        <f t="shared" si="1"/>
+        <v>8.4379453584551811</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>4786145278</v>
       </c>
       <c r="B112" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J112">
+        <f t="shared" si="1"/>
+        <v>4.4574451427906752</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>2225969621</v>
       </c>
       <c r="B113" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J113">
+        <f t="shared" si="1"/>
+        <v>2.0730957584455609</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>7268820096</v>
       </c>
       <c r="B114" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J114">
+        <f t="shared" si="1"/>
+        <v>6.7696162462234497</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>4000788035</v>
       </c>
       <c r="B115" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J115">
+        <f t="shared" si="1"/>
+        <v>3.7260242132470012</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>1820258900</v>
       </c>
       <c r="B116" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J116">
+        <f t="shared" si="1"/>
+        <v>1.6952482052147388</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>12054018540</v>
       </c>
       <c r="B117" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J117">
+        <f t="shared" si="1"/>
+        <v>11.226179581135511</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>7038257254</v>
       </c>
       <c r="B118" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J118">
+        <f t="shared" si="1"/>
+        <v>6.5548878666013479</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>4656480191</v>
       </c>
       <c r="B119" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J119">
+        <f t="shared" si="1"/>
+        <v>4.3366851201280951</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>10050331879</v>
       </c>
       <c r="B120" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J120">
+        <f t="shared" si="1"/>
+        <v>9.3601009612902999</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>6908773272</v>
+        <v>2513965439</v>
       </c>
       <c r="B121" t="s">
         <v>321</v>
+      </c>
+      <c r="J121">
+        <f t="shared" si="1"/>
+        <v>2.3413127651438117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DATABASE: fixed wrong database entries
</commit_message>
<xml_diff>
--- a/resources/database/data/anime/db_anime - staging data.xlsx
+++ b/resources/database/data/anime/db_anime - staging data.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3789" uniqueCount="668">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3791" uniqueCount="668">
   <si>
     <t>Summer</t>
   </si>
@@ -2037,7 +2037,7 @@
     <t>One Piece</t>
   </si>
   <si>
-    <t>NULL</t>
+    <t>0000-00-00</t>
   </si>
 </sst>
 </file>
@@ -2507,10 +2507,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA245"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A230" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A233" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="D249" sqref="D249"/>
+      <selection pane="bottomLeft" activeCell="B246" sqref="A246:XFD246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10278,6 +10278,9 @@
       <c r="J118" t="s">
         <v>123</v>
       </c>
+      <c r="L118" t="s">
+        <v>665</v>
+      </c>
       <c r="N118" s="9" t="s">
         <v>275</v>
       </c>
@@ -18438,10 +18441,13 @@
         <v>4831397928</v>
       </c>
       <c r="I244">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J244" t="s">
-        <v>665</v>
+        <v>123</v>
+      </c>
+      <c r="K244" t="s">
+        <v>123</v>
       </c>
       <c r="N244" s="9" t="s">
         <v>667</v>

</xml_diff>

<commit_message>
DATABASE: added new data for R - Z,
</commit_message>
<xml_diff>
--- a/resources/database/data/anime/db_anime - staging data.xlsx
+++ b/resources/database/data/anime/db_anime - staging data.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3791" uniqueCount="668">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3820" uniqueCount="680">
   <si>
     <t>Summer</t>
   </si>
@@ -2037,7 +2037,43 @@
     <t>One Piece</t>
   </si>
   <si>
+    <t>ReZero kara Hajimeru Isekai Seikatsu</t>
+  </si>
+  <si>
     <t>0000-00-00</t>
+  </si>
+  <si>
+    <t>Re:Zero kara Hajimeru Isekai Seikatsu</t>
+  </si>
+  <si>
+    <t>2017-08-27</t>
+  </si>
+  <si>
+    <t>Tokyo Ravens</t>
+  </si>
+  <si>
+    <t>2017-08-25</t>
+  </si>
+  <si>
+    <t>Spirited Away</t>
+  </si>
+  <si>
+    <t>2017-09-21</t>
+  </si>
+  <si>
+    <t>Yuru Yuri San Hai!</t>
+  </si>
+  <si>
+    <t>2017-08-15</t>
+  </si>
+  <si>
+    <t>World Trigger</t>
+  </si>
+  <si>
+    <t>2016-12-29</t>
+  </si>
+  <si>
+    <t>Project-GXS</t>
   </si>
 </sst>
 </file>
@@ -2117,7 +2153,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2148,6 +2184,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -2505,12 +2542,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA245"/>
+  <dimension ref="A1:AA250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A233" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A228" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="B246" sqref="A246:XFD246"/>
+      <selection pane="bottomLeft" activeCell="D246" sqref="D246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2520,7 +2557,7 @@
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="23.7109375" customWidth="1"/>
-    <col min="14" max="14" width="12.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" style="14" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="9.140625" style="11"/>
@@ -2566,7 +2603,7 @@
       <c r="M1" t="s">
         <v>644</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="14" t="s">
         <v>645</v>
       </c>
       <c r="O1" t="s">
@@ -2643,7 +2680,7 @@
       <c r="L3" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c r="N3" s="14" t="s">
         <v>165</v>
       </c>
       <c r="O3" s="2" t="s">
@@ -2716,7 +2753,7 @@
       <c r="K4" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="N4" s="14" t="s">
         <v>166</v>
       </c>
       <c r="O4" s="2"/>
@@ -2781,7 +2818,7 @@
       <c r="J5" t="s">
         <v>10</v>
       </c>
-      <c r="N5" s="9" t="s">
+      <c r="N5" s="14" t="s">
         <v>167</v>
       </c>
       <c r="O5" s="2" t="s">
@@ -2853,7 +2890,7 @@
       <c r="J6" t="s">
         <v>11</v>
       </c>
-      <c r="N6" s="9" t="s">
+      <c r="N6" s="14" t="s">
         <v>168</v>
       </c>
       <c r="O6" s="2"/>
@@ -2920,7 +2957,7 @@
       <c r="J7" t="s">
         <v>12</v>
       </c>
-      <c r="N7" s="9" t="s">
+      <c r="N7" s="14" t="s">
         <v>169</v>
       </c>
       <c r="O7" s="2" t="s">
@@ -2995,7 +3032,7 @@
       <c r="K8" t="s">
         <v>54</v>
       </c>
-      <c r="N8" s="9" t="s">
+      <c r="N8" s="14" t="s">
         <v>170</v>
       </c>
       <c r="O8" s="2" t="s">
@@ -3054,7 +3091,7 @@
       <c r="J9" t="s">
         <v>14</v>
       </c>
-      <c r="N9" s="9" t="s">
+      <c r="N9" s="14" t="s">
         <v>171</v>
       </c>
       <c r="O9" s="2" t="s">
@@ -3127,7 +3164,7 @@
       <c r="K10" t="s">
         <v>64</v>
       </c>
-      <c r="N10" s="9" t="s">
+      <c r="N10" s="14" t="s">
         <v>172</v>
       </c>
       <c r="O10" s="2" t="s">
@@ -3198,7 +3235,7 @@
       <c r="K11" t="s">
         <v>82</v>
       </c>
-      <c r="N11" s="9" t="s">
+      <c r="N11" s="14" t="s">
         <v>173</v>
       </c>
       <c r="O11" s="2"/>
@@ -3263,7 +3300,7 @@
       <c r="J12" t="s">
         <v>17</v>
       </c>
-      <c r="N12" s="9" t="s">
+      <c r="N12" s="14" t="s">
         <v>174</v>
       </c>
       <c r="O12" s="2" t="s">
@@ -3331,7 +3368,7 @@
       <c r="J13" t="s">
         <v>18</v>
       </c>
-      <c r="N13" s="9" t="s">
+      <c r="N13" s="14" t="s">
         <v>175</v>
       </c>
       <c r="O13" s="2" t="s">
@@ -3399,7 +3436,7 @@
       <c r="J14" t="s">
         <v>19</v>
       </c>
-      <c r="N14" s="9" t="s">
+      <c r="N14" s="14" t="s">
         <v>176</v>
       </c>
       <c r="O14" s="2" t="s">
@@ -3472,7 +3509,7 @@
       <c r="L15" t="s">
         <v>21</v>
       </c>
-      <c r="N15" s="9" t="s">
+      <c r="N15" s="14" t="s">
         <v>177</v>
       </c>
       <c r="O15" s="2" t="s">
@@ -3545,7 +3582,7 @@
       <c r="K16" t="s">
         <v>20</v>
       </c>
-      <c r="N16" s="9" t="s">
+      <c r="N16" s="14" t="s">
         <v>178</v>
       </c>
       <c r="O16" s="2"/>
@@ -3610,7 +3647,7 @@
       <c r="J17" t="s">
         <v>22</v>
       </c>
-      <c r="N17" s="9" t="s">
+      <c r="N17" s="14" t="s">
         <v>179</v>
       </c>
       <c r="O17" s="2" t="s">
@@ -3683,7 +3720,7 @@
       <c r="L18" t="s">
         <v>24</v>
       </c>
-      <c r="N18" s="9" t="s">
+      <c r="N18" s="14" t="s">
         <v>180</v>
       </c>
       <c r="O18" s="2" t="s">
@@ -3756,7 +3793,7 @@
       <c r="K19" t="s">
         <v>23</v>
       </c>
-      <c r="N19" s="9" t="s">
+      <c r="N19" s="14" t="s">
         <v>181</v>
       </c>
       <c r="O19" s="2" t="s">
@@ -3828,7 +3865,7 @@
       <c r="J20" t="s">
         <v>25</v>
       </c>
-      <c r="N20" s="9" t="s">
+      <c r="N20" s="14" t="s">
         <v>182</v>
       </c>
       <c r="O20" s="2" t="s">
@@ -3900,7 +3937,7 @@
       <c r="J21" t="s">
         <v>26</v>
       </c>
-      <c r="N21" s="9" t="s">
+      <c r="N21" s="14" t="s">
         <v>183</v>
       </c>
       <c r="O21" s="2" t="s">
@@ -3968,7 +4005,7 @@
       <c r="J22" t="s">
         <v>27</v>
       </c>
-      <c r="N22" s="9" t="s">
+      <c r="N22" s="14" t="s">
         <v>184</v>
       </c>
       <c r="O22" s="2"/>
@@ -4033,7 +4070,7 @@
       <c r="J23" t="s">
         <v>28</v>
       </c>
-      <c r="N23" s="9" t="s">
+      <c r="N23" s="14" t="s">
         <v>185</v>
       </c>
       <c r="O23" s="2" t="s">
@@ -4104,7 +4141,7 @@
       <c r="K24" t="s">
         <v>99</v>
       </c>
-      <c r="N24" s="9" t="s">
+      <c r="N24" s="14" t="s">
         <v>186</v>
       </c>
       <c r="O24" s="2" t="s">
@@ -4176,7 +4213,7 @@
       <c r="J25" t="s">
         <v>30</v>
       </c>
-      <c r="N25" s="9" t="s">
+      <c r="N25" s="14" t="s">
         <v>187</v>
       </c>
       <c r="O25" s="2" t="s">
@@ -4248,7 +4285,7 @@
       <c r="J26" t="s">
         <v>31</v>
       </c>
-      <c r="N26" s="9" t="s">
+      <c r="N26" s="14" t="s">
         <v>188</v>
       </c>
       <c r="O26" s="2" t="s">
@@ -4320,7 +4357,7 @@
       <c r="J27" t="s">
         <v>32</v>
       </c>
-      <c r="N27" s="9" t="s">
+      <c r="N27" s="14" t="s">
         <v>189</v>
       </c>
       <c r="O27" s="2" t="s">
@@ -4390,7 +4427,7 @@
       <c r="J28" t="s">
         <v>33</v>
       </c>
-      <c r="N28" s="9" t="s">
+      <c r="N28" s="14" t="s">
         <v>190</v>
       </c>
       <c r="O28" s="2"/>
@@ -4453,7 +4490,7 @@
       <c r="J29" t="s">
         <v>34</v>
       </c>
-      <c r="N29" s="9" t="s">
+      <c r="N29" s="14" t="s">
         <v>191</v>
       </c>
       <c r="O29" s="2"/>
@@ -4516,7 +4553,7 @@
       <c r="J30" t="s">
         <v>35</v>
       </c>
-      <c r="N30" s="9" t="s">
+      <c r="N30" s="14" t="s">
         <v>192</v>
       </c>
       <c r="O30" s="2"/>
@@ -4581,7 +4618,7 @@
       <c r="J31" t="s">
         <v>36</v>
       </c>
-      <c r="N31" s="9" t="s">
+      <c r="N31" s="14" t="s">
         <v>193</v>
       </c>
       <c r="O31" s="2"/>
@@ -4646,7 +4683,7 @@
       <c r="J32" t="s">
         <v>37</v>
       </c>
-      <c r="N32" s="9" t="s">
+      <c r="N32" s="14" t="s">
         <v>194</v>
       </c>
       <c r="O32" s="2"/>
@@ -4709,7 +4746,7 @@
       <c r="J33" t="s">
         <v>38</v>
       </c>
-      <c r="N33" s="9" t="s">
+      <c r="N33" s="14" t="s">
         <v>195</v>
       </c>
       <c r="O33" s="2" t="s">
@@ -4777,7 +4814,7 @@
       <c r="J34" t="s">
         <v>39</v>
       </c>
-      <c r="N34" s="9" t="s">
+      <c r="N34" s="14" t="s">
         <v>196</v>
       </c>
       <c r="O34" s="2" t="s">
@@ -4845,7 +4882,7 @@
       <c r="J35" t="s">
         <v>40</v>
       </c>
-      <c r="N35" s="9" t="s">
+      <c r="N35" s="14" t="s">
         <v>197</v>
       </c>
       <c r="O35" s="2"/>
@@ -4908,7 +4945,7 @@
       <c r="J36" t="s">
         <v>41</v>
       </c>
-      <c r="N36" s="9" t="s">
+      <c r="N36" s="14" t="s">
         <v>198</v>
       </c>
       <c r="O36" s="2" t="s">
@@ -4978,7 +5015,7 @@
       <c r="J37" t="s">
         <v>42</v>
       </c>
-      <c r="N37" s="9" t="s">
+      <c r="N37" s="14" t="s">
         <v>199</v>
       </c>
       <c r="O37" s="2"/>
@@ -5041,7 +5078,7 @@
       <c r="J38" t="s">
         <v>43</v>
       </c>
-      <c r="N38" s="9" t="s">
+      <c r="N38" s="14" t="s">
         <v>200</v>
       </c>
       <c r="O38" s="2"/>
@@ -5104,7 +5141,7 @@
       <c r="J39" t="s">
         <v>44</v>
       </c>
-      <c r="N39" s="9" t="s">
+      <c r="N39" s="14" t="s">
         <v>201</v>
       </c>
       <c r="O39" s="2" t="s">
@@ -5172,7 +5209,7 @@
       <c r="J40" t="s">
         <v>45</v>
       </c>
-      <c r="N40" s="9" t="s">
+      <c r="N40" s="14" t="s">
         <v>202</v>
       </c>
       <c r="O40" s="2" t="s">
@@ -5243,7 +5280,7 @@
       <c r="L41" t="s">
         <v>47</v>
       </c>
-      <c r="N41" s="9" t="s">
+      <c r="N41" s="14" t="s">
         <v>203</v>
       </c>
       <c r="O41" s="2"/>
@@ -5309,7 +5346,7 @@
       <c r="K42" t="s">
         <v>46</v>
       </c>
-      <c r="N42" s="9" t="s">
+      <c r="N42" s="14" t="s">
         <v>204</v>
       </c>
       <c r="O42" s="2"/>
@@ -5372,7 +5409,7 @@
       <c r="J43" t="s">
         <v>48</v>
       </c>
-      <c r="N43" s="9" t="s">
+      <c r="N43" s="14" t="s">
         <v>205</v>
       </c>
       <c r="O43" s="2" t="s">
@@ -5440,7 +5477,7 @@
       <c r="J44" t="s">
         <v>49</v>
       </c>
-      <c r="N44" s="9" t="s">
+      <c r="N44" s="14" t="s">
         <v>206</v>
       </c>
       <c r="O44" s="2" t="s">
@@ -5512,7 +5549,7 @@
       <c r="J45" t="s">
         <v>50</v>
       </c>
-      <c r="N45" s="9" t="s">
+      <c r="N45" s="14" t="s">
         <v>207</v>
       </c>
       <c r="O45" s="2" t="s">
@@ -5571,7 +5608,7 @@
       <c r="J46" t="s">
         <v>51</v>
       </c>
-      <c r="N46" s="9" t="s">
+      <c r="N46" s="14" t="s">
         <v>208</v>
       </c>
       <c r="O46" s="2" t="s">
@@ -5639,7 +5676,7 @@
       <c r="J47" t="s">
         <v>52</v>
       </c>
-      <c r="N47" s="9" t="s">
+      <c r="N47" s="14" t="s">
         <v>209</v>
       </c>
       <c r="O47" s="2"/>
@@ -5702,7 +5739,7 @@
       <c r="J48" t="s">
         <v>53</v>
       </c>
-      <c r="N48" s="9" t="s">
+      <c r="N48" s="14" t="s">
         <v>210</v>
       </c>
       <c r="O48" s="2" t="s">
@@ -5767,7 +5804,7 @@
       <c r="M49" t="s">
         <v>13</v>
       </c>
-      <c r="N49" s="9" t="s">
+      <c r="N49" s="14" t="s">
         <v>211</v>
       </c>
       <c r="O49" s="2" t="s">
@@ -5838,7 +5875,7 @@
       <c r="K50" t="s">
         <v>54</v>
       </c>
-      <c r="N50" s="9" t="s">
+      <c r="N50" s="14" t="s">
         <v>212</v>
       </c>
       <c r="O50" s="2" t="s">
@@ -5906,7 +5943,7 @@
       <c r="J51" t="s">
         <v>56</v>
       </c>
-      <c r="N51" s="9" t="s">
+      <c r="N51" s="14" t="s">
         <v>213</v>
       </c>
       <c r="O51" s="2" t="s">
@@ -5968,7 +6005,7 @@
       <c r="L52" t="s">
         <v>660</v>
       </c>
-      <c r="N52" s="9" t="s">
+      <c r="N52" s="14" t="s">
         <v>214</v>
       </c>
       <c r="O52" s="2" t="s">
@@ -6039,7 +6076,7 @@
       <c r="K53" t="s">
         <v>659</v>
       </c>
-      <c r="N53" s="9" t="s">
+      <c r="N53" s="14" t="s">
         <v>215</v>
       </c>
       <c r="O53" s="2" t="s">
@@ -6107,7 +6144,7 @@
       <c r="J54" t="s">
         <v>59</v>
       </c>
-      <c r="N54" s="9" t="s">
+      <c r="N54" s="14" t="s">
         <v>216</v>
       </c>
       <c r="O54" s="2" t="s">
@@ -6175,7 +6212,7 @@
       <c r="J55" t="s">
         <v>60</v>
       </c>
-      <c r="N55" s="9" t="s">
+      <c r="N55" s="14" t="s">
         <v>217</v>
       </c>
       <c r="Q55">
@@ -6239,7 +6276,7 @@
       <c r="J56" t="s">
         <v>61</v>
       </c>
-      <c r="N56" s="9" t="s">
+      <c r="N56" s="14" t="s">
         <v>181</v>
       </c>
       <c r="O56" s="2" t="s">
@@ -6310,7 +6347,7 @@
       <c r="L57" t="s">
         <v>63</v>
       </c>
-      <c r="N57" s="9" t="s">
+      <c r="N57" s="14" t="s">
         <v>218</v>
       </c>
       <c r="O57" s="2" t="s">
@@ -6381,7 +6418,7 @@
       <c r="K58" t="s">
         <v>62</v>
       </c>
-      <c r="N58" s="9" t="s">
+      <c r="N58" s="14" t="s">
         <v>219</v>
       </c>
       <c r="O58" s="2" t="s">
@@ -6452,7 +6489,7 @@
       <c r="L59" t="s">
         <v>15</v>
       </c>
-      <c r="N59" s="9" t="s">
+      <c r="N59" s="14" t="s">
         <v>220</v>
       </c>
       <c r="O59" s="2" t="s">
@@ -6520,7 +6557,7 @@
       <c r="J60" t="s">
         <v>65</v>
       </c>
-      <c r="N60" s="9" t="s">
+      <c r="N60" s="14" t="s">
         <v>221</v>
       </c>
       <c r="O60" s="2" t="s">
@@ -6594,7 +6631,7 @@
       <c r="J61" t="s">
         <v>66</v>
       </c>
-      <c r="N61" s="9" t="s">
+      <c r="N61" s="14" t="s">
         <v>222</v>
       </c>
       <c r="O61" s="2" t="s">
@@ -6664,7 +6701,7 @@
       <c r="J62" t="s">
         <v>67</v>
       </c>
-      <c r="N62" s="9" t="s">
+      <c r="N62" s="14" t="s">
         <v>223</v>
       </c>
       <c r="O62" s="2" t="s">
@@ -6732,7 +6769,7 @@
       <c r="J63" t="s">
         <v>68</v>
       </c>
-      <c r="N63" s="9" t="s">
+      <c r="N63" s="14" t="s">
         <v>224</v>
       </c>
       <c r="O63" s="2"/>
@@ -6797,7 +6834,7 @@
       <c r="J64" t="s">
         <v>69</v>
       </c>
-      <c r="N64" s="9" t="s">
+      <c r="N64" s="14" t="s">
         <v>225</v>
       </c>
       <c r="O64" s="2"/>
@@ -6860,7 +6897,7 @@
       <c r="J65" t="s">
         <v>70</v>
       </c>
-      <c r="N65" s="9" t="s">
+      <c r="N65" s="14" t="s">
         <v>226</v>
       </c>
       <c r="O65" s="2" t="s">
@@ -6919,7 +6956,7 @@
       <c r="J66" t="s">
         <v>71</v>
       </c>
-      <c r="N66" s="9" t="s">
+      <c r="N66" s="14" t="s">
         <v>227</v>
       </c>
       <c r="O66" s="2" t="s">
@@ -6987,7 +7024,7 @@
       <c r="J67" t="s">
         <v>72</v>
       </c>
-      <c r="N67" s="9" t="s">
+      <c r="N67" s="14" t="s">
         <v>228</v>
       </c>
       <c r="O67" s="2" t="s">
@@ -7057,7 +7094,7 @@
       <c r="J68" t="s">
         <v>73</v>
       </c>
-      <c r="N68" s="9" t="s">
+      <c r="N68" s="14" t="s">
         <v>229</v>
       </c>
       <c r="O68" s="2" t="s">
@@ -7130,7 +7167,7 @@
       <c r="L69" t="s">
         <v>75</v>
       </c>
-      <c r="N69" s="9" t="s">
+      <c r="N69" s="14" t="s">
         <v>230</v>
       </c>
       <c r="O69" s="2" t="s">
@@ -7201,7 +7238,7 @@
       <c r="K70" t="s">
         <v>74</v>
       </c>
-      <c r="N70" s="9" t="s">
+      <c r="N70" s="14" t="s">
         <v>231</v>
       </c>
       <c r="O70" s="2"/>
@@ -7264,7 +7301,7 @@
       <c r="J71" t="s">
         <v>76</v>
       </c>
-      <c r="N71" s="9" t="s">
+      <c r="N71" s="14" t="s">
         <v>172</v>
       </c>
       <c r="O71" s="2"/>
@@ -7327,7 +7364,7 @@
       <c r="J72" t="s">
         <v>77</v>
       </c>
-      <c r="N72" s="9" t="s">
+      <c r="N72" s="14" t="s">
         <v>232</v>
       </c>
       <c r="O72" s="2" t="s">
@@ -7398,7 +7435,7 @@
       <c r="L73" t="s">
         <v>79</v>
       </c>
-      <c r="N73" s="9" t="s">
+      <c r="N73" s="14" t="s">
         <v>233</v>
       </c>
       <c r="O73" s="2" t="s">
@@ -7469,7 +7506,7 @@
       <c r="K74" t="s">
         <v>78</v>
       </c>
-      <c r="N74" s="9" t="s">
+      <c r="N74" s="14" t="s">
         <v>234</v>
       </c>
       <c r="O74" s="2"/>
@@ -7532,7 +7569,7 @@
       <c r="J75" t="s">
         <v>80</v>
       </c>
-      <c r="N75" s="9" t="s">
+      <c r="N75" s="14" t="s">
         <v>235</v>
       </c>
       <c r="O75" s="2"/>
@@ -7598,7 +7635,7 @@
       <c r="L76" t="s">
         <v>83</v>
       </c>
-      <c r="N76" s="9" t="s">
+      <c r="N76" s="14" t="s">
         <v>218</v>
       </c>
       <c r="O76" s="2"/>
@@ -7667,7 +7704,7 @@
       <c r="L77" t="s">
         <v>16</v>
       </c>
-      <c r="N77" s="9" t="s">
+      <c r="N77" s="14" t="s">
         <v>236</v>
       </c>
       <c r="O77" s="2"/>
@@ -7738,7 +7775,7 @@
       <c r="L78" t="s">
         <v>82</v>
       </c>
-      <c r="N78" s="9" t="s">
+      <c r="N78" s="14" t="s">
         <v>237</v>
       </c>
       <c r="O78" s="2"/>
@@ -7803,7 +7840,7 @@
       <c r="J79" t="s">
         <v>84</v>
       </c>
-      <c r="N79" s="9" t="s">
+      <c r="N79" s="14" t="s">
         <v>238</v>
       </c>
       <c r="O79" s="2" t="s">
@@ -7873,7 +7910,7 @@
       <c r="J80" t="s">
         <v>85</v>
       </c>
-      <c r="N80" s="9" t="s">
+      <c r="N80" s="14" t="s">
         <v>239</v>
       </c>
       <c r="O80" s="2" t="s">
@@ -7941,7 +7978,7 @@
       <c r="J81" t="s">
         <v>86</v>
       </c>
-      <c r="N81" s="9" t="s">
+      <c r="N81" s="14" t="s">
         <v>240</v>
       </c>
       <c r="O81" s="2" t="s">
@@ -8007,7 +8044,7 @@
       <c r="J82" t="s">
         <v>87</v>
       </c>
-      <c r="N82" s="9" t="s">
+      <c r="N82" s="14" t="s">
         <v>241</v>
       </c>
       <c r="O82" s="2" t="s">
@@ -8077,7 +8114,7 @@
       <c r="J83" t="s">
         <v>88</v>
       </c>
-      <c r="N83" s="9" t="s">
+      <c r="N83" s="14" t="s">
         <v>242</v>
       </c>
       <c r="O83" s="2" t="s">
@@ -8152,7 +8189,7 @@
       <c r="L84" t="s">
         <v>91</v>
       </c>
-      <c r="N84" s="9" t="s">
+      <c r="N84" s="14" t="s">
         <v>243</v>
       </c>
       <c r="O84" s="2"/>
@@ -8220,7 +8257,7 @@
       <c r="K85" t="s">
         <v>91</v>
       </c>
-      <c r="N85" s="9" t="s">
+      <c r="N85" s="14" t="s">
         <v>244</v>
       </c>
       <c r="O85" s="2"/>
@@ -8291,7 +8328,7 @@
       <c r="L86" t="s">
         <v>90</v>
       </c>
-      <c r="N86" s="9" t="s">
+      <c r="N86" s="14" t="s">
         <v>245</v>
       </c>
       <c r="O86" s="2"/>
@@ -8359,7 +8396,7 @@
       <c r="L87" t="s">
         <v>93</v>
       </c>
-      <c r="N87" s="9" t="s">
+      <c r="N87" s="14" t="s">
         <v>246</v>
       </c>
       <c r="O87" s="2"/>
@@ -8425,7 +8462,7 @@
       <c r="K88" t="s">
         <v>92</v>
       </c>
-      <c r="N88" s="9" t="s">
+      <c r="N88" s="14" t="s">
         <v>247</v>
       </c>
       <c r="O88" s="2"/>
@@ -8488,7 +8525,7 @@
       <c r="J89" t="s">
         <v>94</v>
       </c>
-      <c r="N89" s="9" t="s">
+      <c r="N89" s="14" t="s">
         <v>248</v>
       </c>
       <c r="O89" s="4" t="s">
@@ -8556,7 +8593,7 @@
       <c r="J90" t="s">
         <v>95</v>
       </c>
-      <c r="N90" s="9" t="s">
+      <c r="N90" s="14" t="s">
         <v>249</v>
       </c>
       <c r="O90" s="2"/>
@@ -8619,7 +8656,7 @@
       <c r="J91" t="s">
         <v>96</v>
       </c>
-      <c r="N91" s="9" t="s">
+      <c r="N91" s="14" t="s">
         <v>250</v>
       </c>
       <c r="O91" s="2" t="s">
@@ -8689,7 +8726,7 @@
       <c r="J92" t="s">
         <v>97</v>
       </c>
-      <c r="N92" s="9" t="s">
+      <c r="N92" s="14" t="s">
         <v>251</v>
       </c>
       <c r="O92" s="2"/>
@@ -8752,7 +8789,7 @@
       <c r="J93" t="s">
         <v>98</v>
       </c>
-      <c r="N93" s="9" t="s">
+      <c r="N93" s="14" t="s">
         <v>252</v>
       </c>
       <c r="O93" s="2"/>
@@ -8820,7 +8857,7 @@
       <c r="L94" t="s">
         <v>29</v>
       </c>
-      <c r="N94" s="9" t="s">
+      <c r="N94" s="14" t="s">
         <v>253</v>
       </c>
       <c r="O94" s="2" t="s">
@@ -8888,7 +8925,7 @@
       <c r="J95" t="s">
         <v>100</v>
       </c>
-      <c r="N95" s="9" t="s">
+      <c r="N95" s="14" t="s">
         <v>254</v>
       </c>
       <c r="O95" s="2"/>
@@ -8951,7 +8988,7 @@
       <c r="J96" t="s">
         <v>101</v>
       </c>
-      <c r="N96" s="9" t="s">
+      <c r="N96" s="14" t="s">
         <v>255</v>
       </c>
       <c r="O96" s="2"/>
@@ -9017,7 +9054,7 @@
       <c r="K97" t="s">
         <v>128</v>
       </c>
-      <c r="N97" s="9" t="s">
+      <c r="N97" s="14" t="s">
         <v>256</v>
       </c>
       <c r="O97" s="2"/>
@@ -9082,7 +9119,7 @@
       <c r="J98" t="s">
         <v>103</v>
       </c>
-      <c r="N98" s="9" t="s">
+      <c r="N98" s="14" t="s">
         <v>255</v>
       </c>
       <c r="O98" s="2" t="s">
@@ -9150,7 +9187,7 @@
       <c r="J99" t="s">
         <v>104</v>
       </c>
-      <c r="N99" s="9" t="s">
+      <c r="N99" s="14" t="s">
         <v>257</v>
       </c>
       <c r="O99" s="2"/>
@@ -9216,7 +9253,7 @@
       <c r="L100" t="s">
         <v>106</v>
       </c>
-      <c r="N100" s="9" t="s">
+      <c r="N100" s="14" t="s">
         <v>258</v>
       </c>
       <c r="O100" s="2" t="s">
@@ -9289,7 +9326,7 @@
       <c r="K101" t="s">
         <v>105</v>
       </c>
-      <c r="N101" s="9" t="s">
+      <c r="N101" s="14" t="s">
         <v>259</v>
       </c>
       <c r="O101" s="2" t="s">
@@ -9359,7 +9396,7 @@
       <c r="J102" t="s">
         <v>107</v>
       </c>
-      <c r="N102" s="9" t="s">
+      <c r="N102" s="14" t="s">
         <v>260</v>
       </c>
       <c r="O102" s="2"/>
@@ -9422,7 +9459,7 @@
       <c r="J103" t="s">
         <v>108</v>
       </c>
-      <c r="N103" s="9" t="s">
+      <c r="N103" s="14" t="s">
         <v>261</v>
       </c>
       <c r="O103" s="2"/>
@@ -9486,7 +9523,7 @@
       <c r="M104" t="s">
         <v>110</v>
       </c>
-      <c r="N104" s="9" t="s">
+      <c r="N104" s="14" t="s">
         <v>262</v>
       </c>
       <c r="O104" s="2"/>
@@ -9543,7 +9580,7 @@
       <c r="K105" t="s">
         <v>109</v>
       </c>
-      <c r="N105" s="9" t="s">
+      <c r="N105" s="14" t="s">
         <v>263</v>
       </c>
       <c r="O105" s="2"/>
@@ -9597,7 +9634,7 @@
       <c r="J106" t="s">
         <v>111</v>
       </c>
-      <c r="N106" s="9" t="s">
+      <c r="N106" s="14" t="s">
         <v>264</v>
       </c>
       <c r="O106" s="2"/>
@@ -9651,7 +9688,7 @@
       <c r="J107" t="s">
         <v>112</v>
       </c>
-      <c r="N107" s="9" t="s">
+      <c r="N107" s="14" t="s">
         <v>265</v>
       </c>
       <c r="O107" s="2"/>
@@ -9712,7 +9749,7 @@
       <c r="J108" t="s">
         <v>113</v>
       </c>
-      <c r="N108" s="9" t="s">
+      <c r="N108" s="14" t="s">
         <v>266</v>
       </c>
       <c r="O108" s="2"/>
@@ -9775,7 +9812,7 @@
       <c r="J109" t="s">
         <v>114</v>
       </c>
-      <c r="N109" s="9" t="s">
+      <c r="N109" s="14" t="s">
         <v>267</v>
       </c>
       <c r="O109" s="2"/>
@@ -9838,7 +9875,7 @@
       <c r="J110" t="s">
         <v>115</v>
       </c>
-      <c r="N110" s="9" t="s">
+      <c r="N110" s="14" t="s">
         <v>268</v>
       </c>
       <c r="O110" s="2"/>
@@ -9890,7 +9927,7 @@
       <c r="J111" t="s">
         <v>116</v>
       </c>
-      <c r="N111" s="9" t="s">
+      <c r="N111" s="14" t="s">
         <v>269</v>
       </c>
       <c r="O111" s="2"/>
@@ -9942,7 +9979,7 @@
       <c r="J112" t="s">
         <v>117</v>
       </c>
-      <c r="N112" s="9" t="s">
+      <c r="N112" s="14" t="s">
         <v>270</v>
       </c>
       <c r="O112" s="2"/>
@@ -9996,7 +10033,7 @@
       <c r="J113" t="s">
         <v>118</v>
       </c>
-      <c r="N113" s="9" t="s">
+      <c r="N113" s="14" t="s">
         <v>271</v>
       </c>
       <c r="O113" s="2"/>
@@ -10048,7 +10085,7 @@
       <c r="J114" t="s">
         <v>119</v>
       </c>
-      <c r="N114" s="9" t="s">
+      <c r="N114" s="14" t="s">
         <v>272</v>
       </c>
       <c r="O114" s="2"/>
@@ -10102,7 +10139,7 @@
       <c r="J115" t="s">
         <v>120</v>
       </c>
-      <c r="N115" s="9" t="s">
+      <c r="N115" s="14" t="s">
         <v>273</v>
       </c>
       <c r="O115" s="2" t="s">
@@ -10161,7 +10198,7 @@
       <c r="J116" t="s">
         <v>121</v>
       </c>
-      <c r="N116" s="9" t="s">
+      <c r="N116" s="14" t="s">
         <v>262</v>
       </c>
       <c r="O116" s="2"/>
@@ -10215,7 +10252,7 @@
       <c r="J117" t="s">
         <v>122</v>
       </c>
-      <c r="N117" s="9" t="s">
+      <c r="N117" s="14" t="s">
         <v>274</v>
       </c>
       <c r="O117" s="2"/>
@@ -10281,7 +10318,7 @@
       <c r="L118" t="s">
         <v>665</v>
       </c>
-      <c r="N118" s="9" t="s">
+      <c r="N118" s="14" t="s">
         <v>275</v>
       </c>
       <c r="O118" s="2"/>
@@ -10342,7 +10379,7 @@
       <c r="J119" t="s">
         <v>124</v>
       </c>
-      <c r="N119" s="9" t="s">
+      <c r="N119" s="14" t="s">
         <v>276</v>
       </c>
       <c r="O119" s="2"/>
@@ -10403,7 +10440,7 @@
       <c r="J120" t="s">
         <v>125</v>
       </c>
-      <c r="N120" s="9" t="s">
+      <c r="N120" s="14" t="s">
         <v>277</v>
       </c>
       <c r="O120" s="2" t="s">
@@ -10471,7 +10508,7 @@
       <c r="J121" t="s">
         <v>126</v>
       </c>
-      <c r="N121" s="9" t="s">
+      <c r="N121" s="14" t="s">
         <v>273</v>
       </c>
       <c r="O121" s="2" t="s">
@@ -10537,7 +10574,7 @@
       <c r="J122" t="s">
         <v>127</v>
       </c>
-      <c r="N122" s="9" t="s">
+      <c r="N122" s="14" t="s">
         <v>278</v>
       </c>
       <c r="O122" s="2" t="s">
@@ -10608,7 +10645,7 @@
       <c r="L123" t="s">
         <v>102</v>
       </c>
-      <c r="N123" s="9" t="s">
+      <c r="N123" s="14" t="s">
         <v>279</v>
       </c>
       <c r="Q123">
@@ -10670,7 +10707,7 @@
       <c r="J124" t="s">
         <v>324</v>
       </c>
-      <c r="N124" s="9" t="s">
+      <c r="N124" s="14" t="s">
         <v>536</v>
       </c>
       <c r="O124" s="2"/>
@@ -10733,7 +10770,7 @@
       <c r="J125" t="s">
         <v>327</v>
       </c>
-      <c r="N125" s="9" t="s">
+      <c r="N125" s="14" t="s">
         <v>537</v>
       </c>
       <c r="O125" s="2" t="s">
@@ -10801,7 +10838,7 @@
       <c r="J126" t="s">
         <v>441</v>
       </c>
-      <c r="N126" s="9" t="s">
+      <c r="N126" s="14" t="s">
         <v>538</v>
       </c>
       <c r="O126" s="2" t="s">
@@ -10866,7 +10903,7 @@
       <c r="J127" t="s">
         <v>334</v>
       </c>
-      <c r="N127" s="9" t="s">
+      <c r="N127" s="14" t="s">
         <v>539</v>
       </c>
       <c r="O127" s="2" t="s">
@@ -10943,7 +10980,7 @@
       <c r="L128" t="s">
         <v>462</v>
       </c>
-      <c r="N128" s="9" t="s">
+      <c r="N128" s="14" t="s">
         <v>540</v>
       </c>
       <c r="O128" s="2" t="s">
@@ -11014,7 +11051,7 @@
       <c r="L129" t="s">
         <v>444</v>
       </c>
-      <c r="N129" s="9" t="s">
+      <c r="N129" s="14" t="s">
         <v>275</v>
       </c>
       <c r="O129" s="2" t="s">
@@ -11082,7 +11119,7 @@
       <c r="K130" t="s">
         <v>443</v>
       </c>
-      <c r="N130" s="9" t="s">
+      <c r="N130" s="14" t="s">
         <v>541</v>
       </c>
       <c r="O130" s="2" t="s">
@@ -11156,7 +11193,7 @@
       <c r="J131" t="s">
         <v>358</v>
       </c>
-      <c r="N131" s="9" t="s">
+      <c r="N131" s="14" t="s">
         <v>542</v>
       </c>
       <c r="O131" s="2" t="s">
@@ -11221,7 +11258,7 @@
       <c r="J132" t="s">
         <v>364</v>
       </c>
-      <c r="N132" s="9" t="s">
+      <c r="N132" s="14" t="s">
         <v>543</v>
       </c>
       <c r="O132" s="2" t="s">
@@ -11295,7 +11332,7 @@
       <c r="L133" t="s">
         <v>446</v>
       </c>
-      <c r="N133" s="9" t="s">
+      <c r="N133" s="14" t="s">
         <v>544</v>
       </c>
       <c r="O133" s="2" t="s">
@@ -11366,7 +11403,7 @@
       <c r="K134" t="s">
         <v>445</v>
       </c>
-      <c r="N134" s="9" t="s">
+      <c r="N134" s="14" t="s">
         <v>545</v>
       </c>
       <c r="O134" s="2"/>
@@ -11435,7 +11472,7 @@
       <c r="L135" t="s">
         <v>508</v>
       </c>
-      <c r="N135" s="9" t="s">
+      <c r="N135" s="14" t="s">
         <v>546</v>
       </c>
       <c r="O135" s="2" t="s">
@@ -11503,7 +11540,7 @@
       <c r="J136" t="s">
         <v>381</v>
       </c>
-      <c r="N136" s="9" t="s">
+      <c r="N136" s="14" t="s">
         <v>547</v>
       </c>
       <c r="O136" s="2" t="s">
@@ -11571,7 +11608,7 @@
       <c r="J137" t="s">
         <v>383</v>
       </c>
-      <c r="N137" s="9" t="s">
+      <c r="N137" s="14" t="s">
         <v>548</v>
       </c>
       <c r="O137" s="2"/>
@@ -11637,7 +11674,7 @@
       <c r="K138" t="s">
         <v>471</v>
       </c>
-      <c r="N138" s="9" t="s">
+      <c r="N138" s="14" t="s">
         <v>549</v>
       </c>
       <c r="O138" s="2"/>
@@ -11688,7 +11725,7 @@
       <c r="J139" t="s">
         <v>395</v>
       </c>
-      <c r="N139" s="9" t="s">
+      <c r="N139" s="14" t="s">
         <v>538</v>
       </c>
       <c r="O139" s="2" t="s">
@@ -11756,7 +11793,7 @@
       <c r="M140" t="s">
         <v>450</v>
       </c>
-      <c r="N140" s="9" t="s">
+      <c r="N140" s="14" t="s">
         <v>550</v>
       </c>
       <c r="O140" s="2" t="s">
@@ -11824,7 +11861,7 @@
       <c r="K141" t="s">
         <v>449</v>
       </c>
-      <c r="N141" s="9" t="s">
+      <c r="N141" s="14" t="s">
         <v>551</v>
       </c>
       <c r="O141" s="2" t="s">
@@ -11898,7 +11935,7 @@
       <c r="L142" t="s">
         <v>452</v>
       </c>
-      <c r="N142" s="9" t="s">
+      <c r="N142" s="14" t="s">
         <v>552</v>
       </c>
       <c r="O142" s="2"/>
@@ -11964,7 +12001,7 @@
       <c r="K143" t="s">
         <v>451</v>
       </c>
-      <c r="N143" s="9" t="s">
+      <c r="N143" s="14" t="s">
         <v>553</v>
       </c>
       <c r="O143" s="2" t="s">
@@ -12035,7 +12072,7 @@
       <c r="J144" t="s">
         <v>414</v>
       </c>
-      <c r="N144" s="9" t="s">
+      <c r="N144" s="14" t="s">
         <v>554</v>
       </c>
       <c r="O144" s="2" t="s">
@@ -12103,7 +12140,7 @@
       <c r="J145" t="s">
         <v>418</v>
       </c>
-      <c r="N145" s="9" t="s">
+      <c r="N145" s="14" t="s">
         <v>179</v>
       </c>
       <c r="O145" s="2" t="s">
@@ -12171,7 +12208,7 @@
       <c r="J146" t="s">
         <v>424</v>
       </c>
-      <c r="N146" s="9" t="s">
+      <c r="N146" s="14" t="s">
         <v>221</v>
       </c>
       <c r="O146" s="2" t="s">
@@ -12239,7 +12276,7 @@
       <c r="J147" t="s">
         <v>429</v>
       </c>
-      <c r="N147" s="9" t="s">
+      <c r="N147" s="14" t="s">
         <v>555</v>
       </c>
       <c r="O147" s="2" t="s">
@@ -12310,7 +12347,7 @@
       <c r="J148" t="s">
         <v>430</v>
       </c>
-      <c r="N148" s="9" t="s">
+      <c r="N148" s="14" t="s">
         <v>556</v>
       </c>
       <c r="O148" s="2" t="s">
@@ -12378,7 +12415,7 @@
       <c r="J149" t="s">
         <v>431</v>
       </c>
-      <c r="N149" s="9" t="s">
+      <c r="N149" s="14" t="s">
         <v>557</v>
       </c>
       <c r="O149" s="2" t="s">
@@ -12437,7 +12474,7 @@
       <c r="L150" t="s">
         <v>483</v>
       </c>
-      <c r="N150" s="9" t="s">
+      <c r="N150" s="14" t="s">
         <v>558</v>
       </c>
       <c r="O150" s="2" t="s">
@@ -12502,7 +12539,7 @@
       <c r="J151" t="s">
         <v>435</v>
       </c>
-      <c r="N151" s="9" t="s">
+      <c r="N151" s="14" t="s">
         <v>559</v>
       </c>
       <c r="O151" s="2" t="s">
@@ -12576,7 +12613,7 @@
       <c r="L152" t="s">
         <v>455</v>
       </c>
-      <c r="N152" s="9" t="s">
+      <c r="N152" s="14" t="s">
         <v>560</v>
       </c>
       <c r="O152" s="2" t="s">
@@ -12644,7 +12681,7 @@
       <c r="K153" t="s">
         <v>454</v>
       </c>
-      <c r="N153" s="9" t="s">
+      <c r="N153" s="14" t="s">
         <v>561</v>
       </c>
       <c r="O153" s="2" t="s">
@@ -12709,7 +12746,7 @@
       <c r="J154" t="s">
         <v>333</v>
       </c>
-      <c r="N154" s="9" t="s">
+      <c r="N154" s="14" t="s">
         <v>562</v>
       </c>
       <c r="O154" s="2" t="s">
@@ -12777,7 +12814,7 @@
       <c r="L155" t="s">
         <v>457</v>
       </c>
-      <c r="N155" s="9" t="s">
+      <c r="N155" s="14" t="s">
         <v>563</v>
       </c>
       <c r="O155" s="2" t="s">
@@ -12845,7 +12882,7 @@
       <c r="K156" t="s">
         <v>456</v>
       </c>
-      <c r="N156" s="9" t="s">
+      <c r="N156" s="14" t="s">
         <v>564</v>
       </c>
       <c r="O156" s="2"/>
@@ -12908,7 +12945,7 @@
       <c r="L157" t="s">
         <v>459</v>
       </c>
-      <c r="N157" s="9" t="s">
+      <c r="N157" s="14" t="s">
         <v>565</v>
       </c>
       <c r="O157" s="2"/>
@@ -12971,7 +13008,7 @@
       <c r="K158" t="s">
         <v>458</v>
       </c>
-      <c r="N158" s="9" t="s">
+      <c r="N158" s="14" t="s">
         <v>566</v>
       </c>
       <c r="O158" s="2"/>
@@ -13031,7 +13068,7 @@
       <c r="J159" t="s">
         <v>340</v>
       </c>
-      <c r="N159" s="9" t="s">
+      <c r="N159" s="14" t="s">
         <v>567</v>
       </c>
       <c r="O159" s="2" t="s">
@@ -13102,7 +13139,7 @@
       <c r="J160" t="s">
         <v>460</v>
       </c>
-      <c r="N160" s="9" t="s">
+      <c r="N160" s="14" t="s">
         <v>568</v>
       </c>
       <c r="O160" s="2" t="s">
@@ -13176,7 +13213,7 @@
       <c r="L161" t="s">
         <v>442</v>
       </c>
-      <c r="N161" s="9" t="s">
+      <c r="N161" s="14" t="s">
         <v>569</v>
       </c>
       <c r="O161" s="2"/>
@@ -13239,7 +13276,7 @@
       <c r="K162" t="s">
         <v>442</v>
       </c>
-      <c r="N162" s="9" t="s">
+      <c r="N162" s="14" t="s">
         <v>570</v>
       </c>
       <c r="O162" s="2" t="s">
@@ -13307,7 +13344,7 @@
       <c r="J163" t="s">
         <v>345</v>
       </c>
-      <c r="N163" s="9" t="s">
+      <c r="N163" s="14" t="s">
         <v>571</v>
       </c>
       <c r="O163" s="2" t="s">
@@ -13372,7 +13409,7 @@
       <c r="J164" t="s">
         <v>346</v>
       </c>
-      <c r="N164" s="9" t="s">
+      <c r="N164" s="14" t="s">
         <v>572</v>
       </c>
       <c r="O164" s="2"/>
@@ -13432,7 +13469,7 @@
       <c r="J165" t="s">
         <v>347</v>
       </c>
-      <c r="N165" s="9" t="s">
+      <c r="N165" s="14" t="s">
         <v>573</v>
       </c>
       <c r="O165" s="2" t="s">
@@ -13497,7 +13534,7 @@
       <c r="J166" t="s">
         <v>348</v>
       </c>
-      <c r="N166" s="9" t="s">
+      <c r="N166" s="14" t="s">
         <v>574</v>
       </c>
       <c r="O166" s="2" t="s">
@@ -13562,7 +13599,7 @@
       <c r="J167" t="s">
         <v>463</v>
       </c>
-      <c r="N167" s="9" t="s">
+      <c r="N167" s="14" t="s">
         <v>575</v>
       </c>
       <c r="O167" s="2"/>
@@ -13625,7 +13662,7 @@
       <c r="J168" t="s">
         <v>354</v>
       </c>
-      <c r="N168" s="9" t="s">
+      <c r="N168" s="14" t="s">
         <v>576</v>
       </c>
       <c r="O168" s="2"/>
@@ -13691,7 +13728,7 @@
       <c r="J169" t="s">
         <v>464</v>
       </c>
-      <c r="N169" s="9" t="s">
+      <c r="N169" s="14" t="s">
         <v>577</v>
       </c>
       <c r="O169" s="2" t="s">
@@ -13768,7 +13805,7 @@
       <c r="M170" t="s">
         <v>662</v>
       </c>
-      <c r="N170" s="9" t="s">
+      <c r="N170" s="14" t="s">
         <v>578</v>
       </c>
       <c r="O170" s="2"/>
@@ -13834,7 +13871,7 @@
       <c r="L171" t="s">
         <v>496</v>
       </c>
-      <c r="N171" s="9" t="s">
+      <c r="N171" s="14" t="s">
         <v>183</v>
       </c>
       <c r="O171" s="2"/>
@@ -13894,7 +13931,7 @@
       <c r="J172" t="s">
         <v>365</v>
       </c>
-      <c r="N172" s="9" t="s">
+      <c r="N172" s="14" t="s">
         <v>579</v>
       </c>
       <c r="O172" s="2" t="s">
@@ -13962,7 +13999,7 @@
       <c r="J173" t="s">
         <v>370</v>
       </c>
-      <c r="N173" s="9" t="s">
+      <c r="N173" s="14" t="s">
         <v>580</v>
       </c>
       <c r="O173" s="2" t="s">
@@ -14039,7 +14076,7 @@
       <c r="K174" t="s">
         <v>447</v>
       </c>
-      <c r="N174" s="9" t="s">
+      <c r="N174" s="14" t="s">
         <v>581</v>
       </c>
       <c r="O174" s="2"/>
@@ -14105,7 +14142,7 @@
       <c r="J175" t="s">
         <v>379</v>
       </c>
-      <c r="N175" s="9" t="s">
+      <c r="N175" s="14" t="s">
         <v>582</v>
       </c>
       <c r="O175" s="2"/>
@@ -14165,7 +14202,7 @@
       <c r="J176" t="s">
         <v>384</v>
       </c>
-      <c r="N176" s="9" t="s">
+      <c r="N176" s="14" t="s">
         <v>583</v>
       </c>
       <c r="O176" s="2" t="s">
@@ -14236,7 +14273,7 @@
       <c r="J177" t="s">
         <v>386</v>
       </c>
-      <c r="N177" s="9" t="s">
+      <c r="N177" s="14" t="s">
         <v>584</v>
       </c>
       <c r="O177" s="2"/>
@@ -14299,7 +14336,7 @@
       <c r="J178" t="s">
         <v>387</v>
       </c>
-      <c r="N178" s="9" t="s">
+      <c r="N178" s="14" t="s">
         <v>585</v>
       </c>
       <c r="O178" s="2" t="s">
@@ -14370,7 +14407,7 @@
       <c r="K179" t="s">
         <v>492</v>
       </c>
-      <c r="N179" s="9" t="s">
+      <c r="N179" s="14" t="s">
         <v>586</v>
       </c>
       <c r="O179" s="2"/>
@@ -14430,7 +14467,7 @@
       <c r="J180" t="s">
         <v>469</v>
       </c>
-      <c r="N180" s="9" t="s">
+      <c r="N180" s="14" t="s">
         <v>587</v>
       </c>
       <c r="O180" s="2"/>
@@ -14493,7 +14530,7 @@
       <c r="K181" t="s">
         <v>471</v>
       </c>
-      <c r="N181" s="9" t="s">
+      <c r="N181" s="14" t="s">
         <v>588</v>
       </c>
       <c r="O181" s="2"/>
@@ -14547,7 +14584,7 @@
       <c r="M182" t="s">
         <v>663</v>
       </c>
-      <c r="N182" s="9" t="s">
+      <c r="N182" s="14" t="s">
         <v>589</v>
       </c>
       <c r="O182" s="2"/>
@@ -14598,7 +14635,7 @@
       <c r="J183" t="s">
         <v>398</v>
       </c>
-      <c r="N183" s="9" t="s">
+      <c r="N183" s="14" t="s">
         <v>590</v>
       </c>
       <c r="O183" s="2" t="s">
@@ -14654,7 +14691,7 @@
       <c r="J184" t="s">
         <v>399</v>
       </c>
-      <c r="N184" s="9" t="s">
+      <c r="N184" s="14" t="s">
         <v>591</v>
       </c>
       <c r="O184" s="2" t="s">
@@ -14722,7 +14759,7 @@
       <c r="L185" t="s">
         <v>473</v>
       </c>
-      <c r="N185" s="9" t="s">
+      <c r="N185" s="14" t="s">
         <v>592</v>
       </c>
       <c r="O185" s="2" t="s">
@@ -14796,7 +14833,7 @@
       <c r="L186" t="s">
         <v>474</v>
       </c>
-      <c r="N186" s="9" t="s">
+      <c r="N186" s="14" t="s">
         <v>252</v>
       </c>
       <c r="O186" s="2" t="s">
@@ -14867,7 +14904,7 @@
       <c r="K187" t="s">
         <v>473</v>
       </c>
-      <c r="N187" s="9" t="s">
+      <c r="N187" s="14" t="s">
         <v>252</v>
       </c>
       <c r="O187" s="2"/>
@@ -14933,7 +14970,7 @@
       <c r="L188" t="s">
         <v>493</v>
       </c>
-      <c r="N188" s="9" t="s">
+      <c r="N188" s="14" t="s">
         <v>593</v>
       </c>
       <c r="O188" s="2" t="s">
@@ -15001,7 +15038,7 @@
       <c r="L189" t="s">
         <v>477</v>
       </c>
-      <c r="N189" s="9" t="s">
+      <c r="N189" s="14" t="s">
         <v>594</v>
       </c>
       <c r="O189" s="2"/>
@@ -15064,7 +15101,7 @@
       <c r="K190" t="s">
         <v>476</v>
       </c>
-      <c r="N190" s="9" t="s">
+      <c r="N190" s="14" t="s">
         <v>595</v>
       </c>
       <c r="O190" s="2" t="s">
@@ -15138,7 +15175,7 @@
       <c r="L191" t="s">
         <v>451</v>
       </c>
-      <c r="N191" s="9" t="s">
+      <c r="N191" s="14" t="s">
         <v>171</v>
       </c>
       <c r="O191" s="2" t="s">
@@ -15212,7 +15249,7 @@
       <c r="M192" t="s">
         <v>481</v>
       </c>
-      <c r="N192" s="9" t="s">
+      <c r="N192" s="14" t="s">
         <v>251</v>
       </c>
       <c r="O192" s="2"/>
@@ -15275,7 +15312,7 @@
       <c r="K193" t="s">
         <v>479</v>
       </c>
-      <c r="N193" s="9" t="s">
+      <c r="N193" s="14" t="s">
         <v>596</v>
       </c>
       <c r="O193" s="2" t="s">
@@ -15343,7 +15380,7 @@
       <c r="K194" t="s">
         <v>479</v>
       </c>
-      <c r="N194" s="9" t="s">
+      <c r="N194" s="14" t="s">
         <v>251</v>
       </c>
       <c r="O194" s="2"/>
@@ -15403,7 +15440,7 @@
       <c r="J195" t="s">
         <v>415</v>
       </c>
-      <c r="N195" s="9" t="s">
+      <c r="N195" s="14" t="s">
         <v>597</v>
       </c>
       <c r="O195" s="2"/>
@@ -15466,7 +15503,7 @@
       <c r="J196" t="s">
         <v>416</v>
       </c>
-      <c r="N196" s="9" t="s">
+      <c r="N196" s="14" t="s">
         <v>598</v>
       </c>
       <c r="O196" s="2" t="s">
@@ -15531,7 +15568,7 @@
       <c r="J197" t="s">
         <v>417</v>
       </c>
-      <c r="N197" s="9" t="s">
+      <c r="N197" s="14" t="s">
         <v>599</v>
       </c>
       <c r="O197" s="2"/>
@@ -15594,7 +15631,7 @@
       <c r="J198" t="s">
         <v>421</v>
       </c>
-      <c r="N198" s="9" t="s">
+      <c r="N198" s="14" t="s">
         <v>600</v>
       </c>
       <c r="O198" s="2" t="s">
@@ -15659,7 +15696,7 @@
       <c r="J199" t="s">
         <v>423</v>
       </c>
-      <c r="N199" s="9" t="s">
+      <c r="N199" s="14" t="s">
         <v>178</v>
       </c>
       <c r="O199" s="2"/>
@@ -15722,7 +15759,7 @@
       <c r="J200" t="s">
         <v>425</v>
       </c>
-      <c r="N200" s="9" t="s">
+      <c r="N200" s="14" t="s">
         <v>601</v>
       </c>
       <c r="O200" s="2" t="s">
@@ -15787,7 +15824,7 @@
       <c r="J201" t="s">
         <v>426</v>
       </c>
-      <c r="N201" s="9" t="s">
+      <c r="N201" s="14" t="s">
         <v>602</v>
       </c>
       <c r="O201" s="2" t="s">
@@ -15855,7 +15892,7 @@
       <c r="K202" t="s">
         <v>505</v>
       </c>
-      <c r="N202" s="9" t="s">
+      <c r="N202" s="14" t="s">
         <v>603</v>
       </c>
       <c r="O202" s="2"/>
@@ -15915,7 +15952,7 @@
       <c r="J203" t="s">
         <v>432</v>
       </c>
-      <c r="N203" s="9" t="s">
+      <c r="N203" s="14" t="s">
         <v>248</v>
       </c>
       <c r="O203" s="2" t="s">
@@ -15983,7 +16020,10 @@
       <c r="K204" t="s">
         <v>453</v>
       </c>
-      <c r="N204" s="9" t="s">
+      <c r="L204" t="s">
+        <v>675</v>
+      </c>
+      <c r="N204" s="14" t="s">
         <v>549</v>
       </c>
       <c r="O204" s="2" t="s">
@@ -16039,7 +16079,7 @@
       <c r="J205" t="s">
         <v>436</v>
       </c>
-      <c r="N205" s="9" t="s">
+      <c r="N205" s="14" t="s">
         <v>604</v>
       </c>
       <c r="O205" s="2"/>
@@ -16102,7 +16142,7 @@
       <c r="L206" t="s">
         <v>485</v>
       </c>
-      <c r="N206" s="9" t="s">
+      <c r="N206" s="14" t="s">
         <v>605</v>
       </c>
       <c r="O206" s="2"/>
@@ -16168,7 +16208,7 @@
       <c r="L207" t="s">
         <v>486</v>
       </c>
-      <c r="N207" s="9" t="s">
+      <c r="N207" s="14" t="s">
         <v>606</v>
       </c>
       <c r="O207" s="2"/>
@@ -16234,7 +16274,7 @@
       <c r="L208" t="s">
         <v>487</v>
       </c>
-      <c r="N208" s="9" t="s">
+      <c r="N208" s="14" t="s">
         <v>607</v>
       </c>
       <c r="O208" s="2"/>
@@ -16297,7 +16337,7 @@
       <c r="K209" t="s">
         <v>486</v>
       </c>
-      <c r="N209" s="9" t="s">
+      <c r="N209" s="14" t="s">
         <v>608</v>
       </c>
       <c r="O209" s="2"/>
@@ -16357,7 +16397,7 @@
       <c r="J210" t="s">
         <v>325</v>
       </c>
-      <c r="N210" s="9" t="s">
+      <c r="N210" s="14" t="s">
         <v>609</v>
       </c>
       <c r="O210" s="2"/>
@@ -16423,7 +16463,7 @@
       <c r="M211" t="s">
         <v>489</v>
       </c>
-      <c r="N211" s="9" t="s">
+      <c r="N211" s="14" t="s">
         <v>610</v>
       </c>
       <c r="O211" s="2"/>
@@ -16486,7 +16526,7 @@
       <c r="K212" t="s">
         <v>488</v>
       </c>
-      <c r="N212" s="9" t="s">
+      <c r="N212" s="14" t="s">
         <v>611</v>
       </c>
       <c r="O212" s="2"/>
@@ -16549,7 +16589,7 @@
       <c r="K213" t="s">
         <v>488</v>
       </c>
-      <c r="N213" s="9" t="s">
+      <c r="N213" s="14" t="s">
         <v>611</v>
       </c>
       <c r="O213" s="2"/>
@@ -16609,7 +16649,7 @@
       <c r="J214" t="s">
         <v>349</v>
       </c>
-      <c r="N214" s="9" t="s">
+      <c r="N214" s="14" t="s">
         <v>245</v>
       </c>
       <c r="O214" s="2"/>
@@ -16675,7 +16715,7 @@
       <c r="K215" t="s">
         <v>465</v>
       </c>
-      <c r="N215" s="9" t="s">
+      <c r="N215" s="14" t="s">
         <v>264</v>
       </c>
       <c r="O215" s="2"/>
@@ -16735,7 +16775,7 @@
       <c r="J216" t="s">
         <v>366</v>
       </c>
-      <c r="N216" s="9" t="s">
+      <c r="N216" s="14" t="s">
         <v>612</v>
       </c>
       <c r="O216" s="2"/>
@@ -16795,7 +16835,7 @@
       <c r="J217" t="s">
         <v>380</v>
       </c>
-      <c r="N217" s="9" t="s">
+      <c r="N217" s="14" t="s">
         <v>613</v>
       </c>
       <c r="O217" s="2"/>
@@ -16858,7 +16898,7 @@
       <c r="L218" t="s">
         <v>468</v>
       </c>
-      <c r="N218" s="9" t="s">
+      <c r="N218" s="14" t="s">
         <v>614</v>
       </c>
       <c r="O218" s="2"/>
@@ -16921,7 +16961,7 @@
       <c r="K219" t="s">
         <v>475</v>
       </c>
-      <c r="N219" s="9" t="s">
+      <c r="N219" s="14" t="s">
         <v>191</v>
       </c>
       <c r="O219" s="2"/>
@@ -16981,7 +17021,7 @@
       <c r="J220" t="s">
         <v>323</v>
       </c>
-      <c r="N220" s="9" t="s">
+      <c r="N220" s="14" t="s">
         <v>615</v>
       </c>
       <c r="O220" s="2" t="s">
@@ -17040,7 +17080,7 @@
       <c r="J221" t="s">
         <v>326</v>
       </c>
-      <c r="N221" s="9" t="s">
+      <c r="N221" s="14" t="s">
         <v>616</v>
       </c>
       <c r="O221" s="2"/>
@@ -17100,7 +17140,7 @@
       <c r="J222" t="s">
         <v>351</v>
       </c>
-      <c r="N222" s="9" t="s">
+      <c r="N222" s="14" t="s">
         <v>262</v>
       </c>
       <c r="O222" s="2" t="s">
@@ -17171,7 +17211,7 @@
       <c r="L223" t="s">
         <v>661</v>
       </c>
-      <c r="N223" s="9" t="s">
+      <c r="N223" s="14" t="s">
         <v>617</v>
       </c>
       <c r="O223" s="2"/>
@@ -17228,7 +17268,7 @@
       <c r="K224" t="s">
         <v>494</v>
       </c>
-      <c r="N224" s="9" t="s">
+      <c r="N224" s="14" t="s">
         <v>618</v>
       </c>
       <c r="O224" s="2" t="s">
@@ -17290,7 +17330,7 @@
       <c r="K225" t="s">
         <v>466</v>
       </c>
-      <c r="N225" s="9" t="s">
+      <c r="N225" s="14" t="s">
         <v>277</v>
       </c>
       <c r="O225" s="2"/>
@@ -17344,7 +17384,7 @@
       <c r="K226" t="s">
         <v>465</v>
       </c>
-      <c r="N226" s="9" t="s">
+      <c r="N226" s="14" t="s">
         <v>619</v>
       </c>
       <c r="O226" s="2"/>
@@ -17398,7 +17438,7 @@
       <c r="K227" t="s">
         <v>465</v>
       </c>
-      <c r="N227" s="9" t="s">
+      <c r="N227" s="14" t="s">
         <v>620</v>
       </c>
       <c r="O227" s="2"/>
@@ -17449,7 +17489,7 @@
       <c r="J228" t="s">
         <v>367</v>
       </c>
-      <c r="N228" s="9" t="s">
+      <c r="N228" s="14" t="s">
         <v>621</v>
       </c>
       <c r="O228" s="2" t="s">
@@ -17517,7 +17557,7 @@
       <c r="L229" t="s">
         <v>509</v>
       </c>
-      <c r="N229" s="9" t="s">
+      <c r="N229" s="14" t="s">
         <v>622</v>
       </c>
       <c r="O229" s="2"/>
@@ -17580,7 +17620,7 @@
       <c r="K230" t="s">
         <v>499</v>
       </c>
-      <c r="N230" s="9" t="s">
+      <c r="N230" s="14" t="s">
         <v>622</v>
       </c>
       <c r="O230" s="2"/>
@@ -17643,7 +17683,7 @@
       <c r="L231" t="s">
         <v>502</v>
       </c>
-      <c r="N231" s="9" t="s">
+      <c r="N231" s="14" t="s">
         <v>623</v>
       </c>
       <c r="O231" s="2"/>
@@ -17712,7 +17752,7 @@
       <c r="L232" t="s">
         <v>503</v>
       </c>
-      <c r="N232" s="9" t="s">
+      <c r="N232" s="14" t="s">
         <v>268</v>
       </c>
       <c r="O232" s="2"/>
@@ -17778,7 +17818,7 @@
       <c r="K233" t="s">
         <v>502</v>
       </c>
-      <c r="N233" s="9" t="s">
+      <c r="N233" s="14" t="s">
         <v>621</v>
       </c>
       <c r="O233" s="2"/>
@@ -17841,7 +17881,7 @@
       <c r="J234" t="s">
         <v>378</v>
       </c>
-      <c r="N234" s="9" t="s">
+      <c r="N234" s="14" t="s">
         <v>624</v>
       </c>
       <c r="O234" s="2" t="s">
@@ -17897,7 +17937,7 @@
       <c r="J235" t="s">
         <v>382</v>
       </c>
-      <c r="N235" s="9" t="s">
+      <c r="N235" s="14" t="s">
         <v>625</v>
       </c>
       <c r="O235" s="2" t="s">
@@ -17962,7 +18002,7 @@
       <c r="J236" t="s">
         <v>385</v>
       </c>
-      <c r="N236" s="9" t="s">
+      <c r="N236" s="14" t="s">
         <v>626</v>
       </c>
       <c r="O236" s="2"/>
@@ -18025,7 +18065,7 @@
       <c r="J237" t="s">
         <v>388</v>
       </c>
-      <c r="N237" s="9" t="s">
+      <c r="N237" s="14" t="s">
         <v>627</v>
       </c>
       <c r="O237" s="2" t="s">
@@ -18084,7 +18124,7 @@
       <c r="J238" t="s">
         <v>400</v>
       </c>
-      <c r="N238" s="9" t="s">
+      <c r="N238" s="14" t="s">
         <v>628</v>
       </c>
       <c r="O238" s="2"/>
@@ -18144,7 +18184,7 @@
       <c r="J239" t="s">
         <v>504</v>
       </c>
-      <c r="N239" s="9" t="s">
+      <c r="N239" s="14" t="s">
         <v>629</v>
       </c>
       <c r="O239" s="2"/>
@@ -18204,7 +18244,7 @@
       <c r="J240" t="s">
         <v>419</v>
       </c>
-      <c r="N240" s="9" t="s">
+      <c r="N240" s="14" t="s">
         <v>630</v>
       </c>
       <c r="O240" s="2"/>
@@ -18264,7 +18304,7 @@
       <c r="J241" t="s">
         <v>420</v>
       </c>
-      <c r="N241" s="9" t="s">
+      <c r="N241" s="14" t="s">
         <v>631</v>
       </c>
       <c r="O241" s="2"/>
@@ -18324,7 +18364,7 @@
       <c r="J242" t="s">
         <v>422</v>
       </c>
-      <c r="N242" s="9" t="s">
+      <c r="N242" s="14" t="s">
         <v>622</v>
       </c>
       <c r="O242" s="2"/>
@@ -18387,7 +18427,7 @@
       <c r="L243" t="s">
         <v>482</v>
       </c>
-      <c r="N243" s="9" t="s">
+      <c r="N243" s="14" t="s">
         <v>271</v>
       </c>
       <c r="O243" s="2" t="s">
@@ -18449,8 +18489,8 @@
       <c r="K244" t="s">
         <v>123</v>
       </c>
-      <c r="N244" s="9" t="s">
-        <v>667</v>
+      <c r="N244" s="14" t="s">
+        <v>668</v>
       </c>
       <c r="W244">
         <v>1</v>
@@ -18499,22 +18539,344 @@
       <c r="J245" t="s">
         <v>666</v>
       </c>
-      <c r="N245" s="9" t="s">
+      <c r="N245" s="14" t="s">
+        <v>668</v>
+      </c>
+      <c r="W245">
+        <v>1</v>
+      </c>
+      <c r="X245">
+        <v>0</v>
+      </c>
+      <c r="Y245">
+        <v>0</v>
+      </c>
+      <c r="Z245">
+        <v>0</v>
+      </c>
+      <c r="AA245">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A246">
+        <v>244</v>
+      </c>
+      <c r="B246">
+        <v>0</v>
+      </c>
+      <c r="C246" t="s">
+        <v>2</v>
+      </c>
+      <c r="D246" t="s">
         <v>667</v>
       </c>
-      <c r="W245">
-        <v>1</v>
-      </c>
-      <c r="X245">
-        <v>0</v>
-      </c>
-      <c r="Y245">
-        <v>0</v>
-      </c>
-      <c r="Z245">
-        <v>0</v>
-      </c>
-      <c r="AA245">
+      <c r="E246">
+        <v>25</v>
+      </c>
+      <c r="F246">
+        <v>0</v>
+      </c>
+      <c r="G246">
+        <v>0</v>
+      </c>
+      <c r="H246">
+        <v>20535137246</v>
+      </c>
+      <c r="I246">
+        <v>1</v>
+      </c>
+      <c r="J246" t="s">
+        <v>667</v>
+      </c>
+      <c r="N246" s="14" t="s">
+        <v>670</v>
+      </c>
+      <c r="Q246">
+        <v>10</v>
+      </c>
+      <c r="R246">
+        <v>40</v>
+      </c>
+      <c r="S246">
+        <v>40</v>
+      </c>
+      <c r="T246" s="11" t="s">
+        <v>521</v>
+      </c>
+      <c r="U246" t="s">
+        <v>669</v>
+      </c>
+      <c r="W246">
+        <v>1</v>
+      </c>
+      <c r="X246">
+        <v>0</v>
+      </c>
+      <c r="Y246">
+        <v>0</v>
+      </c>
+      <c r="Z246">
+        <v>0</v>
+      </c>
+      <c r="AA246">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A247">
+        <v>245</v>
+      </c>
+      <c r="B247">
+        <v>0</v>
+      </c>
+      <c r="C247" t="s">
+        <v>2</v>
+      </c>
+      <c r="D247" t="s">
+        <v>671</v>
+      </c>
+      <c r="E247">
+        <v>24</v>
+      </c>
+      <c r="F247">
+        <v>0</v>
+      </c>
+      <c r="G247">
+        <v>0</v>
+      </c>
+      <c r="H247">
+        <v>39510945127</v>
+      </c>
+      <c r="I247">
+        <v>1</v>
+      </c>
+      <c r="J247" t="s">
+        <v>671</v>
+      </c>
+      <c r="N247" s="14" t="s">
+        <v>672</v>
+      </c>
+      <c r="O247" t="s">
+        <v>3</v>
+      </c>
+      <c r="P247">
+        <v>2013</v>
+      </c>
+      <c r="Q247">
+        <v>9</v>
+      </c>
+      <c r="R247">
+        <v>28</v>
+      </c>
+      <c r="S247">
+        <v>4</v>
+      </c>
+      <c r="T247" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="W247">
+        <v>1</v>
+      </c>
+      <c r="X247">
+        <v>0</v>
+      </c>
+      <c r="Y247">
+        <v>0</v>
+      </c>
+      <c r="Z247">
+        <v>0</v>
+      </c>
+      <c r="AA247">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A248">
+        <v>246</v>
+      </c>
+      <c r="B248">
+        <v>0</v>
+      </c>
+      <c r="C248" t="s">
+        <v>2</v>
+      </c>
+      <c r="D248" t="s">
+        <v>673</v>
+      </c>
+      <c r="E248">
+        <v>1</v>
+      </c>
+      <c r="F248">
+        <v>0</v>
+      </c>
+      <c r="G248">
+        <v>0</v>
+      </c>
+      <c r="H248">
+        <v>14918758264</v>
+      </c>
+      <c r="I248">
+        <v>1</v>
+      </c>
+      <c r="J248" t="s">
+        <v>673</v>
+      </c>
+      <c r="N248" s="14" t="s">
+        <v>674</v>
+      </c>
+      <c r="Q248">
+        <v>2</v>
+      </c>
+      <c r="R248">
+        <v>4</v>
+      </c>
+      <c r="S248">
+        <v>32</v>
+      </c>
+      <c r="T248" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="W248">
+        <v>1</v>
+      </c>
+      <c r="X248">
+        <v>0</v>
+      </c>
+      <c r="Y248">
+        <v>0</v>
+      </c>
+      <c r="Z248">
+        <v>0</v>
+      </c>
+      <c r="AA248">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A249">
+        <v>247</v>
+      </c>
+      <c r="B249">
+        <v>0</v>
+      </c>
+      <c r="C249" t="s">
+        <v>2</v>
+      </c>
+      <c r="D249" t="s">
+        <v>675</v>
+      </c>
+      <c r="E249">
+        <v>12</v>
+      </c>
+      <c r="F249">
+        <v>0</v>
+      </c>
+      <c r="G249">
+        <v>0</v>
+      </c>
+      <c r="H249">
+        <v>9890052998</v>
+      </c>
+      <c r="I249">
+        <v>3</v>
+      </c>
+      <c r="J249" t="s">
+        <v>453</v>
+      </c>
+      <c r="K249" t="s">
+        <v>483</v>
+      </c>
+      <c r="N249" s="14" t="s">
+        <v>676</v>
+      </c>
+      <c r="Q249">
+        <v>4</v>
+      </c>
+      <c r="R249">
+        <v>47</v>
+      </c>
+      <c r="S249">
+        <v>15</v>
+      </c>
+      <c r="T249" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="W249">
+        <v>1</v>
+      </c>
+      <c r="X249">
+        <v>0</v>
+      </c>
+      <c r="Y249">
+        <v>0</v>
+      </c>
+      <c r="Z249">
+        <v>0</v>
+      </c>
+      <c r="AA249">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A250">
+        <v>248</v>
+      </c>
+      <c r="B250">
+        <v>0</v>
+      </c>
+      <c r="C250" t="s">
+        <v>4</v>
+      </c>
+      <c r="D250" t="s">
+        <v>677</v>
+      </c>
+      <c r="E250">
+        <v>73</v>
+      </c>
+      <c r="F250">
+        <v>0</v>
+      </c>
+      <c r="G250">
+        <v>0</v>
+      </c>
+      <c r="H250">
+        <v>9236555666</v>
+      </c>
+      <c r="I250">
+        <v>1</v>
+      </c>
+      <c r="J250" t="s">
+        <v>677</v>
+      </c>
+      <c r="N250" s="14" t="s">
+        <v>678</v>
+      </c>
+      <c r="Q250">
+        <v>28</v>
+      </c>
+      <c r="R250">
+        <v>11</v>
+      </c>
+      <c r="S250">
+        <v>34</v>
+      </c>
+      <c r="T250" s="11" t="s">
+        <v>679</v>
+      </c>
+      <c r="W250">
+        <v>1</v>
+      </c>
+      <c r="X250">
+        <v>0</v>
+      </c>
+      <c r="Y250">
+        <v>0</v>
+      </c>
+      <c r="Z250">
+        <v>0</v>
+      </c>
+      <c r="AA250">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DATABASE: fixed invalid character, exported the updated version of the database to csv format
</commit_message>
<xml_diff>
--- a/resources/database/data/anime/db_anime - staging data.xlsx
+++ b/resources/database/data/anime/db_anime - staging data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4200" windowWidth="24000" windowHeight="9495" tabRatio="856"/>
+    <workbookView xWindow="0" yWindow="4800" windowWidth="24000" windowHeight="9495" tabRatio="856"/>
   </bookViews>
   <sheets>
     <sheet name="&gt;&gt;Final" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5387" uniqueCount="935">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5387" uniqueCount="936">
   <si>
     <t>Summer</t>
   </si>
@@ -2840,6 +2840,9 @@
   </si>
   <si>
     <t>2014-06-04</t>
+  </si>
+  <si>
+    <t>Ikoku Meiro no Croisee</t>
   </si>
 </sst>
 </file>
@@ -3315,10 +3318,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA381"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A295" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A361" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="L267" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="F378" sqref="F378"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28237,7 +28240,7 @@
         <v>7</v>
       </c>
       <c r="D375" t="s">
-        <v>923</v>
+        <v>935</v>
       </c>
       <c r="E375" s="15">
         <v>12</v>
@@ -28255,7 +28258,7 @@
         <v>1</v>
       </c>
       <c r="J375" t="s">
-        <v>923</v>
+        <v>935</v>
       </c>
       <c r="N375" s="14" t="s">
         <v>924</v>

</xml_diff>

<commit_message>
DATABASE: fixed wrong titles
</commit_message>
<xml_diff>
--- a/resources/database/data/anime/db_anime - staging data.xlsx
+++ b/resources/database/data/anime/db_anime - staging data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5400" windowWidth="24000" windowHeight="9495" tabRatio="856"/>
+    <workbookView xWindow="0" yWindow="6000" windowWidth="24000" windowHeight="9495" tabRatio="856"/>
   </bookViews>
   <sheets>
     <sheet name="&gt;&gt;Final" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4741" uniqueCount="974">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4741" uniqueCount="976">
   <si>
     <t>Summer</t>
   </si>
@@ -2957,6 +2957,12 @@
   </si>
   <si>
     <t>A Silent Voice</t>
+  </si>
+  <si>
+    <t>Honeyworks - Zutto Mae Kara Suki Deshita</t>
+  </si>
+  <si>
+    <t>Honeyworks - Suki ni Naru Sono Shunkan wo</t>
   </si>
 </sst>
 </file>
@@ -3438,9 +3444,9 @@
   <dimension ref="A1:AA269"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A233" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="D250" sqref="A3:AA269"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20617,7 +20623,7 @@
         <v>2</v>
       </c>
       <c r="D263" t="s">
-        <v>960</v>
+        <v>974</v>
       </c>
       <c r="E263">
         <v>1</v>
@@ -20685,7 +20691,7 @@
         <v>2</v>
       </c>
       <c r="D264" t="s">
-        <v>959</v>
+        <v>975</v>
       </c>
       <c r="E264">
         <v>1</v>

</xml_diff>

<commit_message>
DATABASE: fixed wrong quality value, exported the updated version of the database
</commit_message>
<xml_diff>
--- a/resources/database/data/anime/db_anime - staging data.xlsx
+++ b/resources/database/data/anime/db_anime - staging data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6600" windowWidth="24000" windowHeight="9495" tabRatio="856"/>
+    <workbookView xWindow="0" yWindow="7800" windowWidth="24000" windowHeight="9495" tabRatio="856"/>
   </bookViews>
   <sheets>
     <sheet name="&gt;&gt;Final" sheetId="1" r:id="rId1"/>
@@ -2971,9 +2971,6 @@
     <t>2017-09-16</t>
   </si>
   <si>
-    <t>UHD 2160p</t>
-  </si>
-  <si>
     <t>Kimi no Na Wa</t>
   </si>
   <si>
@@ -3035,6 +3032,9 @@
   </si>
   <si>
     <t>Nanatsu no Taizai</t>
+  </si>
+  <si>
+    <t>4K 2160p</t>
   </si>
 </sst>
 </file>
@@ -3518,10 +3518,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA280"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A266" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A257" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="T275" sqref="T275"/>
+      <selection pane="bottomLeft" activeCell="C273" sqref="C273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6581,7 +6581,7 @@
         <v>51</v>
       </c>
       <c r="N46" s="14" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="O46" s="2" t="s">
         <v>0</v>
@@ -6599,7 +6599,7 @@
         <v>7</v>
       </c>
       <c r="T46" s="1" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="U46" s="7"/>
       <c r="V46" s="7"/>
@@ -20829,7 +20829,7 @@
         <v>960</v>
       </c>
       <c r="M265" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="N265" s="14" t="s">
         <v>537</v>
@@ -21251,10 +21251,10 @@
         <v>0</v>
       </c>
       <c r="C272" t="s">
+        <v>999</v>
+      </c>
+      <c r="D272" t="s">
         <v>978</v>
-      </c>
-      <c r="D272" t="s">
-        <v>979</v>
       </c>
       <c r="E272">
         <v>1</v>
@@ -21266,10 +21266,10 @@
         <v>1</v>
       </c>
       <c r="J272" t="s">
+        <v>978</v>
+      </c>
+      <c r="N272" s="14" t="s">
         <v>979</v>
-      </c>
-      <c r="N272" s="14" t="s">
-        <v>980</v>
       </c>
       <c r="Q272">
         <v>1</v>
@@ -21281,10 +21281,10 @@
         <v>35</v>
       </c>
       <c r="T272" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="U272" s="11" t="s">
         <v>993</v>
-      </c>
-      <c r="U272" s="11" t="s">
-        <v>994</v>
       </c>
       <c r="W272">
         <v>1</v>
@@ -21313,7 +21313,7 @@
         <v>4</v>
       </c>
       <c r="D273" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="E273">
         <v>10</v>
@@ -21325,13 +21325,13 @@
         <v>1</v>
       </c>
       <c r="J273" t="s">
+        <v>980</v>
+      </c>
+      <c r="L273" t="s">
         <v>981</v>
       </c>
-      <c r="L273" t="s">
+      <c r="N273" s="14" t="s">
         <v>982</v>
-      </c>
-      <c r="N273" s="14" t="s">
-        <v>983</v>
       </c>
       <c r="Q273">
         <v>3</v>
@@ -21346,7 +21346,7 @@
         <v>135</v>
       </c>
       <c r="U273" s="11" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="V273" t="s">
         <v>2</v>
@@ -21378,7 +21378,7 @@
         <v>4</v>
       </c>
       <c r="D274" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="E274">
         <v>11</v>
@@ -21390,10 +21390,10 @@
         <v>2</v>
       </c>
       <c r="J274" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="K274" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="N274" s="14" t="s">
         <v>948</v>
@@ -21408,7 +21408,7 @@
         <v>58</v>
       </c>
       <c r="U274" s="11" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="V274" t="s">
         <v>2</v>
@@ -21440,7 +21440,7 @@
         <v>4</v>
       </c>
       <c r="D275" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="E275">
         <v>12</v>
@@ -21455,13 +21455,13 @@
         <v>1</v>
       </c>
       <c r="J275" t="s">
+        <v>985</v>
+      </c>
+      <c r="L275" t="s">
         <v>986</v>
       </c>
-      <c r="L275" t="s">
+      <c r="N275" s="14" t="s">
         <v>987</v>
-      </c>
-      <c r="N275" s="14" t="s">
-        <v>988</v>
       </c>
       <c r="Q275">
         <v>5</v>
@@ -21499,7 +21499,7 @@
         <v>4</v>
       </c>
       <c r="D276" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="E276">
         <v>12</v>
@@ -21511,13 +21511,13 @@
         <v>2</v>
       </c>
       <c r="J276" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="K276" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="N276" s="14" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="O276" t="s">
         <v>3</v>
@@ -21561,7 +21561,7 @@
         <v>4</v>
       </c>
       <c r="D277" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="E277">
         <v>1</v>
@@ -21620,7 +21620,7 @@
         <v>2</v>
       </c>
       <c r="D278" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="E278">
         <v>12</v>
@@ -21635,7 +21635,7 @@
         <v>1</v>
       </c>
       <c r="J278" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="N278" s="14" t="s">
         <v>935</v>
@@ -21650,7 +21650,7 @@
         <v>33</v>
       </c>
       <c r="T278" s="1" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="W278">
         <v>1</v>
@@ -21679,7 +21679,7 @@
         <v>2</v>
       </c>
       <c r="D279" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="E279">
         <v>13</v>
@@ -21691,10 +21691,10 @@
         <v>1</v>
       </c>
       <c r="J279" t="s">
+        <v>996</v>
+      </c>
+      <c r="N279" s="14" t="s">
         <v>997</v>
-      </c>
-      <c r="N279" s="14" t="s">
-        <v>998</v>
       </c>
       <c r="O279" t="s">
         <v>131</v>
@@ -21741,7 +21741,7 @@
         <v>2</v>
       </c>
       <c r="D280" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="E280">
         <v>24</v>
@@ -21753,7 +21753,7 @@
         <v>1</v>
       </c>
       <c r="J280" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="N280" s="14" t="s">
         <v>941</v>

</xml_diff>

<commit_message>
DATABASE: added 12 entries for staging data, modified 3 entries
</commit_message>
<xml_diff>
--- a/resources/database/data/anime/db_anime - staging data.xlsx
+++ b/resources/database/data/anime/db_anime - staging data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7800" windowWidth="24000" windowHeight="9495" tabRatio="856"/>
+    <workbookView xWindow="0" yWindow="9000" windowWidth="24000" windowHeight="9495" tabRatio="856"/>
   </bookViews>
   <sheets>
     <sheet name="&gt;&gt;Final" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4807" uniqueCount="1000">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4951" uniqueCount="1044">
   <si>
     <t>Summer</t>
   </si>
@@ -3035,6 +3035,138 @@
   </si>
   <si>
     <t>4K 2160p</t>
+  </si>
+  <si>
+    <t>2017-11-07</t>
+  </si>
+  <si>
+    <t>3-gatsu no Lion</t>
+  </si>
+  <si>
+    <t>2017-09-07</t>
+  </si>
+  <si>
+    <t>2017-09-28</t>
+  </si>
+  <si>
+    <t>Chuunibyou demo Koi ga Shitai! The Movie</t>
+  </si>
+  <si>
+    <t>Chuunibyou demo Koi ga Shitai! The Movie Lite</t>
+  </si>
+  <si>
+    <t>FTW</t>
+  </si>
+  <si>
+    <t>D-Frag!</t>
+  </si>
+  <si>
+    <t>2017-09-15</t>
+  </si>
+  <si>
+    <t>God Eater</t>
+  </si>
+  <si>
+    <t>2017-05-05</t>
+  </si>
+  <si>
+    <t>BD 720p</t>
+  </si>
+  <si>
+    <t>Kuroshitsuji</t>
+  </si>
+  <si>
+    <t>2017-01-02</t>
+  </si>
+  <si>
+    <t>Black Buttler</t>
+  </si>
+  <si>
+    <t>Kuzu no Honkai</t>
+  </si>
+  <si>
+    <t>2017-07-08</t>
+  </si>
+  <si>
+    <t>Mikakunin de Shinkoukei</t>
+  </si>
+  <si>
+    <t>2017-09-25</t>
+  </si>
+  <si>
+    <t>Engaged to the Unidentified</t>
+  </si>
+  <si>
+    <t>Nanatsu no Taizai - Seisen no Shirushi</t>
+  </si>
+  <si>
+    <t>Bakemono</t>
+  </si>
+  <si>
+    <t>Nanatsu no Taizai - Signs of Holy War</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Orange Mirai</t>
+  </si>
+  <si>
+    <t>2017-11-08</t>
+  </si>
+  <si>
+    <t>2017-08-03</t>
+  </si>
+  <si>
+    <t>Kokashi</t>
+  </si>
+  <si>
+    <t>Persona 3 Movie 1 - Spring of Birth</t>
+  </si>
+  <si>
+    <t>Persona 3 Movie 2 - Midsummer Knight's Dream</t>
+  </si>
+  <si>
+    <t>Persona 3 Movie 3 - Falling Down</t>
+  </si>
+  <si>
+    <t>Persona 3 Movie 4 - Winter of Rebirth</t>
+  </si>
+  <si>
+    <t>2016-12-30</t>
+  </si>
+  <si>
+    <t>Rakudai Kishi no Cavalry</t>
+  </si>
+  <si>
+    <t>2017-09-14</t>
+  </si>
+  <si>
+    <t>Servamp</t>
+  </si>
+  <si>
+    <t>2017-10-01</t>
+  </si>
+  <si>
+    <t>Ore ga Ojousama Gakkou ni "Shomin Sample" Toshite Gets Sareta Ken</t>
+  </si>
+  <si>
+    <t>2017-09-20</t>
+  </si>
+  <si>
+    <t>Sword Art Online II</t>
+  </si>
+  <si>
+    <t>2017-04-04</t>
+  </si>
+  <si>
+    <t>2017-09-22</t>
+  </si>
+  <si>
+    <t>Watashi ga Motete Dousunda</t>
+  </si>
+  <si>
+    <t>2017-09-03</t>
   </si>
 </sst>
 </file>
@@ -3516,18 +3648,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA280"/>
+  <dimension ref="A1:AA302"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A257" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A275" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="C273" sqref="C273"/>
+      <selection pane="bottomLeft" activeCell="D283" sqref="D283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="56.7109375" customWidth="1"/>
+    <col min="4" max="4" width="73.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="49.7109375" customWidth="1"/>
     <col min="11" max="13" width="23.7109375" customWidth="1"/>
@@ -12680,6 +12812,9 @@
       <c r="J139" t="s">
         <v>393</v>
       </c>
+      <c r="L139" t="s">
+        <v>1039</v>
+      </c>
       <c r="N139" s="14" t="s">
         <v>536</v>
       </c>
@@ -18934,7 +19069,7 @@
         <v>0</v>
       </c>
       <c r="C236" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D236" t="s">
         <v>383</v>
@@ -18949,7 +19084,7 @@
         <v>0</v>
       </c>
       <c r="H236">
-        <v>1308831115</v>
+        <v>2782145536</v>
       </c>
       <c r="I236">
         <v>1</v>
@@ -18958,7 +19093,7 @@
         <v>383</v>
       </c>
       <c r="N236" s="14" t="s">
-        <v>624</v>
+        <v>1038</v>
       </c>
       <c r="O236" s="2"/>
       <c r="Q236">
@@ -18970,8 +19105,8 @@
       <c r="S236">
         <v>57</v>
       </c>
-      <c r="V236" t="s">
-        <v>4</v>
+      <c r="T236" s="1" t="s">
+        <v>677</v>
       </c>
       <c r="W236">
         <v>1</v>
@@ -19068,10 +19203,10 @@
         <v>0</v>
       </c>
       <c r="G238">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H238">
-        <v>730883652</v>
+        <v>2227065587</v>
       </c>
       <c r="I238">
         <v>1</v>
@@ -19080,17 +19215,20 @@
         <v>398</v>
       </c>
       <c r="N238" s="14" t="s">
-        <v>626</v>
+        <v>1041</v>
       </c>
       <c r="O238" s="2"/>
       <c r="Q238">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R238">
+        <v>7</v>
+      </c>
+      <c r="S238">
         <v>32</v>
       </c>
-      <c r="S238">
-        <v>14</v>
+      <c r="T238" s="1" t="s">
+        <v>677</v>
       </c>
       <c r="W238">
         <v>1</v>
@@ -21746,8 +21884,11 @@
       <c r="E280">
         <v>24</v>
       </c>
+      <c r="F280">
+        <v>2</v>
+      </c>
       <c r="H280">
-        <v>16627119198</v>
+        <v>17173320152</v>
       </c>
       <c r="I280">
         <v>1</v>
@@ -21755,8 +21896,11 @@
       <c r="J280" t="s">
         <v>998</v>
       </c>
+      <c r="L280" t="s">
+        <v>1020</v>
+      </c>
       <c r="N280" s="14" t="s">
-        <v>941</v>
+        <v>1000</v>
       </c>
       <c r="O280" t="s">
         <v>130</v>
@@ -21765,10 +21909,10 @@
         <v>2014</v>
       </c>
       <c r="Q280">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R280">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="S280">
         <v>21</v>
@@ -21786,6 +21930,1367 @@
         <v>0</v>
       </c>
       <c r="AA280">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A281">
+        <v>279</v>
+      </c>
+      <c r="B281">
+        <v>0</v>
+      </c>
+      <c r="C281" t="s">
+        <v>4</v>
+      </c>
+      <c r="D281" t="s">
+        <v>814</v>
+      </c>
+      <c r="E281">
+        <v>37</v>
+      </c>
+      <c r="H281">
+        <v>8519257107</v>
+      </c>
+      <c r="I281">
+        <v>1</v>
+      </c>
+      <c r="J281" t="s">
+        <v>814</v>
+      </c>
+      <c r="N281" s="14" t="s">
+        <v>1000</v>
+      </c>
+      <c r="O281" t="s">
+        <v>130</v>
+      </c>
+      <c r="P281">
+        <v>2006</v>
+      </c>
+      <c r="Q281">
+        <v>14</v>
+      </c>
+      <c r="R281">
+        <v>9</v>
+      </c>
+      <c r="S281">
+        <v>11</v>
+      </c>
+      <c r="T281" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="W281">
+        <v>1</v>
+      </c>
+      <c r="X281">
+        <v>0</v>
+      </c>
+      <c r="Y281">
+        <v>0</v>
+      </c>
+      <c r="Z281">
+        <v>0</v>
+      </c>
+      <c r="AA281">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A282">
+        <v>280</v>
+      </c>
+      <c r="B282">
+        <v>0</v>
+      </c>
+      <c r="C282" t="s">
+        <v>4</v>
+      </c>
+      <c r="D282" t="s">
+        <v>1001</v>
+      </c>
+      <c r="E282">
+        <v>22</v>
+      </c>
+      <c r="H282">
+        <v>6539796249</v>
+      </c>
+      <c r="I282">
+        <v>1</v>
+      </c>
+      <c r="J282" t="s">
+        <v>1001</v>
+      </c>
+      <c r="N282" s="14" t="s">
+        <v>1002</v>
+      </c>
+      <c r="Q282">
+        <v>9</v>
+      </c>
+      <c r="R282">
+        <v>35</v>
+      </c>
+      <c r="S282">
+        <v>11</v>
+      </c>
+      <c r="T282" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="W282">
+        <v>1</v>
+      </c>
+      <c r="X282">
+        <v>0</v>
+      </c>
+      <c r="Y282">
+        <v>0</v>
+      </c>
+      <c r="Z282">
+        <v>0</v>
+      </c>
+      <c r="AA282">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A283">
+        <v>281</v>
+      </c>
+      <c r="B283">
+        <v>0</v>
+      </c>
+      <c r="C283" t="s">
+        <v>5</v>
+      </c>
+      <c r="D283" t="s">
+        <v>751</v>
+      </c>
+      <c r="E283">
+        <v>26</v>
+      </c>
+      <c r="H283">
+        <v>3349508624</v>
+      </c>
+      <c r="I283">
+        <v>1</v>
+      </c>
+      <c r="J283" t="s">
+        <v>751</v>
+      </c>
+      <c r="N283" s="14" t="s">
+        <v>1003</v>
+      </c>
+      <c r="O283" t="s">
+        <v>130</v>
+      </c>
+      <c r="P283">
+        <v>2007</v>
+      </c>
+      <c r="Q283">
+        <v>10</v>
+      </c>
+      <c r="R283">
+        <v>33</v>
+      </c>
+      <c r="S283">
+        <v>9</v>
+      </c>
+      <c r="T283" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="W283">
+        <v>1</v>
+      </c>
+      <c r="X283">
+        <v>0</v>
+      </c>
+      <c r="Y283">
+        <v>0</v>
+      </c>
+      <c r="Z283">
+        <v>0</v>
+      </c>
+      <c r="AA283">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A284">
+        <v>282</v>
+      </c>
+      <c r="B284">
+        <v>0</v>
+      </c>
+      <c r="C284" t="s">
+        <v>4</v>
+      </c>
+      <c r="D284" t="s">
+        <v>1004</v>
+      </c>
+      <c r="E284">
+        <v>1</v>
+      </c>
+      <c r="H284">
+        <v>1936365890</v>
+      </c>
+      <c r="I284">
+        <v>0</v>
+      </c>
+      <c r="J284" t="s">
+        <v>788</v>
+      </c>
+      <c r="K284" t="s">
+        <v>788</v>
+      </c>
+      <c r="N284" s="14" t="s">
+        <v>975</v>
+      </c>
+      <c r="Q284">
+        <v>1</v>
+      </c>
+      <c r="R284">
+        <v>30</v>
+      </c>
+      <c r="S284">
+        <v>0</v>
+      </c>
+      <c r="T284" s="1" t="s">
+        <v>1006</v>
+      </c>
+      <c r="W284">
+        <v>1</v>
+      </c>
+      <c r="X284">
+        <v>0</v>
+      </c>
+      <c r="Y284">
+        <v>0</v>
+      </c>
+      <c r="Z284">
+        <v>0</v>
+      </c>
+      <c r="AA284">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A285">
+        <v>283</v>
+      </c>
+      <c r="B285">
+        <v>0</v>
+      </c>
+      <c r="C285" t="s">
+        <v>4</v>
+      </c>
+      <c r="D285" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E285">
+        <v>1</v>
+      </c>
+      <c r="H285">
+        <v>118126284</v>
+      </c>
+      <c r="I285">
+        <v>0</v>
+      </c>
+      <c r="J285" t="s">
+        <v>788</v>
+      </c>
+      <c r="K285" t="s">
+        <v>788</v>
+      </c>
+      <c r="N285" s="14" t="s">
+        <v>975</v>
+      </c>
+      <c r="Q285">
+        <v>0</v>
+      </c>
+      <c r="R285">
+        <v>5</v>
+      </c>
+      <c r="S285">
+        <v>37</v>
+      </c>
+      <c r="T285" s="1" t="s">
+        <v>1006</v>
+      </c>
+      <c r="W285">
+        <v>1</v>
+      </c>
+      <c r="X285">
+        <v>0</v>
+      </c>
+      <c r="Y285">
+        <v>0</v>
+      </c>
+      <c r="Z285">
+        <v>0</v>
+      </c>
+      <c r="AA285">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A286">
+        <v>284</v>
+      </c>
+      <c r="B286">
+        <v>0</v>
+      </c>
+      <c r="C286" t="s">
+        <v>4</v>
+      </c>
+      <c r="D286" t="s">
+        <v>1007</v>
+      </c>
+      <c r="E286">
+        <v>12</v>
+      </c>
+      <c r="F286">
+        <v>1</v>
+      </c>
+      <c r="H286">
+        <v>1631400541</v>
+      </c>
+      <c r="I286">
+        <v>1</v>
+      </c>
+      <c r="J286" t="s">
+        <v>1007</v>
+      </c>
+      <c r="N286" s="14" t="s">
+        <v>1008</v>
+      </c>
+      <c r="O286" t="s">
+        <v>3</v>
+      </c>
+      <c r="P286">
+        <v>2014</v>
+      </c>
+      <c r="Q286">
+        <v>5</v>
+      </c>
+      <c r="R286">
+        <v>10</v>
+      </c>
+      <c r="S286">
+        <v>13</v>
+      </c>
+      <c r="T286" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="W286">
+        <v>1</v>
+      </c>
+      <c r="X286">
+        <v>0</v>
+      </c>
+      <c r="Y286">
+        <v>0</v>
+      </c>
+      <c r="Z286">
+        <v>0</v>
+      </c>
+      <c r="AA286">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A287">
+        <v>285</v>
+      </c>
+      <c r="B287">
+        <v>0</v>
+      </c>
+      <c r="C287" t="s">
+        <v>4</v>
+      </c>
+      <c r="D287" t="s">
+        <v>1009</v>
+      </c>
+      <c r="E287">
+        <v>13</v>
+      </c>
+      <c r="F287">
+        <v>1</v>
+      </c>
+      <c r="H287">
+        <v>2262965412</v>
+      </c>
+      <c r="I287">
+        <v>1</v>
+      </c>
+      <c r="J287" t="s">
+        <v>1009</v>
+      </c>
+      <c r="N287" s="14" t="s">
+        <v>1010</v>
+      </c>
+      <c r="O287" t="s">
+        <v>0</v>
+      </c>
+      <c r="P287">
+        <v>2015</v>
+      </c>
+      <c r="Q287">
+        <v>5</v>
+      </c>
+      <c r="R287">
+        <v>21</v>
+      </c>
+      <c r="S287">
+        <v>25</v>
+      </c>
+      <c r="V287" t="s">
+        <v>1011</v>
+      </c>
+      <c r="W287">
+        <v>1</v>
+      </c>
+      <c r="X287">
+        <v>0</v>
+      </c>
+      <c r="Y287">
+        <v>0</v>
+      </c>
+      <c r="Z287">
+        <v>0</v>
+      </c>
+      <c r="AA287">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A288">
+        <v>286</v>
+      </c>
+      <c r="B288">
+        <v>0</v>
+      </c>
+      <c r="C288" t="s">
+        <v>4</v>
+      </c>
+      <c r="D288" t="s">
+        <v>1012</v>
+      </c>
+      <c r="E288">
+        <v>10</v>
+      </c>
+      <c r="H288">
+        <v>1302075919</v>
+      </c>
+      <c r="I288">
+        <v>1</v>
+      </c>
+      <c r="J288" t="s">
+        <v>1012</v>
+      </c>
+      <c r="N288" s="14" t="s">
+        <v>1013</v>
+      </c>
+      <c r="Q288">
+        <v>4</v>
+      </c>
+      <c r="R288">
+        <v>1</v>
+      </c>
+      <c r="S288">
+        <v>56</v>
+      </c>
+      <c r="T288" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="U288" s="11" t="s">
+        <v>1014</v>
+      </c>
+      <c r="W288">
+        <v>1</v>
+      </c>
+      <c r="X288">
+        <v>0</v>
+      </c>
+      <c r="Y288">
+        <v>0</v>
+      </c>
+      <c r="Z288">
+        <v>0</v>
+      </c>
+      <c r="AA288">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A289">
+        <v>287</v>
+      </c>
+      <c r="B289">
+        <v>0</v>
+      </c>
+      <c r="C289" t="s">
+        <v>4</v>
+      </c>
+      <c r="D289" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E289">
+        <v>12</v>
+      </c>
+      <c r="H289">
+        <v>4041223453</v>
+      </c>
+      <c r="I289">
+        <v>1</v>
+      </c>
+      <c r="J289" t="s">
+        <v>1015</v>
+      </c>
+      <c r="N289" s="14" t="s">
+        <v>1016</v>
+      </c>
+      <c r="Q289">
+        <v>4</v>
+      </c>
+      <c r="R289">
+        <v>35</v>
+      </c>
+      <c r="S289">
+        <v>0</v>
+      </c>
+      <c r="T289" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="W289">
+        <v>1</v>
+      </c>
+      <c r="X289">
+        <v>0</v>
+      </c>
+      <c r="Y289">
+        <v>0</v>
+      </c>
+      <c r="Z289">
+        <v>0</v>
+      </c>
+      <c r="AA289">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A290">
+        <v>288</v>
+      </c>
+      <c r="B290">
+        <v>0</v>
+      </c>
+      <c r="C290" t="s">
+        <v>4</v>
+      </c>
+      <c r="D290" t="s">
+        <v>1017</v>
+      </c>
+      <c r="E290">
+        <v>12</v>
+      </c>
+      <c r="H290">
+        <v>3832297436</v>
+      </c>
+      <c r="I290">
+        <v>1</v>
+      </c>
+      <c r="J290" t="s">
+        <v>1017</v>
+      </c>
+      <c r="N290" s="14" t="s">
+        <v>1018</v>
+      </c>
+      <c r="O290" t="s">
+        <v>3</v>
+      </c>
+      <c r="P290">
+        <v>2014</v>
+      </c>
+      <c r="Q290">
+        <v>4</v>
+      </c>
+      <c r="R290">
+        <v>44</v>
+      </c>
+      <c r="S290">
+        <v>9</v>
+      </c>
+      <c r="T290" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="U290" s="11" t="s">
+        <v>1019</v>
+      </c>
+      <c r="W290">
+        <v>1</v>
+      </c>
+      <c r="X290">
+        <v>0</v>
+      </c>
+      <c r="Y290">
+        <v>0</v>
+      </c>
+      <c r="Z290">
+        <v>0</v>
+      </c>
+      <c r="AA290">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A291">
+        <v>289</v>
+      </c>
+      <c r="B291">
+        <v>0</v>
+      </c>
+      <c r="C291" t="s">
+        <v>4</v>
+      </c>
+      <c r="D291" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E291">
+        <v>4</v>
+      </c>
+      <c r="H291">
+        <v>1634279712</v>
+      </c>
+      <c r="I291">
+        <v>2</v>
+      </c>
+      <c r="J291" t="s">
+        <v>998</v>
+      </c>
+      <c r="K291" t="s">
+        <v>998</v>
+      </c>
+      <c r="N291" s="14" t="s">
+        <v>1000</v>
+      </c>
+      <c r="O291" t="s">
+        <v>0</v>
+      </c>
+      <c r="P291">
+        <v>2016</v>
+      </c>
+      <c r="Q291">
+        <v>1</v>
+      </c>
+      <c r="R291">
+        <v>36</v>
+      </c>
+      <c r="S291">
+        <v>59</v>
+      </c>
+      <c r="T291" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="U291" s="11" t="s">
+        <v>1022</v>
+      </c>
+      <c r="W291">
+        <v>1</v>
+      </c>
+      <c r="X291">
+        <v>0</v>
+      </c>
+      <c r="Y291">
+        <v>0</v>
+      </c>
+      <c r="Z291">
+        <v>0</v>
+      </c>
+      <c r="AA291">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A292">
+        <v>290</v>
+      </c>
+      <c r="B292">
+        <v>0</v>
+      </c>
+      <c r="C292" t="s">
+        <v>4</v>
+      </c>
+      <c r="D292" t="s">
+        <v>1023</v>
+      </c>
+      <c r="E292">
+        <v>13</v>
+      </c>
+      <c r="H292">
+        <v>4600470484</v>
+      </c>
+      <c r="I292">
+        <v>1</v>
+      </c>
+      <c r="J292" t="s">
+        <v>1023</v>
+      </c>
+      <c r="M292" t="s">
+        <v>1024</v>
+      </c>
+      <c r="N292" s="14" t="s">
+        <v>1026</v>
+      </c>
+      <c r="O292" t="s">
+        <v>0</v>
+      </c>
+      <c r="P292">
+        <v>2016</v>
+      </c>
+      <c r="Q292">
+        <v>5</v>
+      </c>
+      <c r="R292">
+        <v>21</v>
+      </c>
+      <c r="S292">
+        <v>57</v>
+      </c>
+      <c r="T292" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="V292" t="s">
+        <v>163</v>
+      </c>
+      <c r="W292">
+        <v>1</v>
+      </c>
+      <c r="X292">
+        <v>0</v>
+      </c>
+      <c r="Y292">
+        <v>0</v>
+      </c>
+      <c r="Z292">
+        <v>0</v>
+      </c>
+      <c r="AA292">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A293">
+        <v>291</v>
+      </c>
+      <c r="B293">
+        <v>0</v>
+      </c>
+      <c r="C293" t="s">
+        <v>4</v>
+      </c>
+      <c r="D293" t="s">
+        <v>1024</v>
+      </c>
+      <c r="E293">
+        <v>13</v>
+      </c>
+      <c r="H293">
+        <v>1432845308</v>
+      </c>
+      <c r="I293">
+        <v>0</v>
+      </c>
+      <c r="J293" t="s">
+        <v>1023</v>
+      </c>
+      <c r="K293" t="s">
+        <v>1023</v>
+      </c>
+      <c r="N293" s="14" t="s">
+        <v>1025</v>
+      </c>
+      <c r="Q293">
+        <v>1</v>
+      </c>
+      <c r="R293">
+        <v>2</v>
+      </c>
+      <c r="S293">
+        <v>5</v>
+      </c>
+      <c r="T293" s="1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="W293">
+        <v>1</v>
+      </c>
+      <c r="X293">
+        <v>0</v>
+      </c>
+      <c r="Y293">
+        <v>0</v>
+      </c>
+      <c r="Z293">
+        <v>0</v>
+      </c>
+      <c r="AA293">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A294">
+        <v>292</v>
+      </c>
+      <c r="B294">
+        <v>0</v>
+      </c>
+      <c r="C294" t="s">
+        <v>4</v>
+      </c>
+      <c r="D294" t="s">
+        <v>1037</v>
+      </c>
+      <c r="E294">
+        <v>12</v>
+      </c>
+      <c r="H294">
+        <v>1452954748</v>
+      </c>
+      <c r="I294">
+        <v>1</v>
+      </c>
+      <c r="J294" t="s">
+        <v>1037</v>
+      </c>
+      <c r="N294" s="14" t="s">
+        <v>971</v>
+      </c>
+      <c r="O294" t="s">
+        <v>130</v>
+      </c>
+      <c r="P294">
+        <v>2015</v>
+      </c>
+      <c r="Q294">
+        <v>4</v>
+      </c>
+      <c r="R294">
+        <v>48</v>
+      </c>
+      <c r="S294">
+        <v>1</v>
+      </c>
+      <c r="T294" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="V294" t="s">
+        <v>532</v>
+      </c>
+      <c r="W294">
+        <v>1</v>
+      </c>
+      <c r="X294">
+        <v>0</v>
+      </c>
+      <c r="Y294">
+        <v>0</v>
+      </c>
+      <c r="Z294">
+        <v>0</v>
+      </c>
+      <c r="AA294">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A295">
+        <v>293</v>
+      </c>
+      <c r="B295">
+        <v>0</v>
+      </c>
+      <c r="C295" t="s">
+        <v>2</v>
+      </c>
+      <c r="D295" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E295">
+        <v>1</v>
+      </c>
+      <c r="H295">
+        <v>1494774022</v>
+      </c>
+      <c r="I295">
+        <v>3</v>
+      </c>
+      <c r="J295" t="s">
+        <v>128</v>
+      </c>
+      <c r="K295" t="s">
+        <v>102</v>
+      </c>
+      <c r="L295" t="s">
+        <v>1029</v>
+      </c>
+      <c r="N295" s="14" t="s">
+        <v>676</v>
+      </c>
+      <c r="Q295">
+        <v>1</v>
+      </c>
+      <c r="R295">
+        <v>38</v>
+      </c>
+      <c r="S295">
+        <v>32</v>
+      </c>
+      <c r="T295" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="W295">
+        <v>1</v>
+      </c>
+      <c r="X295">
+        <v>0</v>
+      </c>
+      <c r="Y295">
+        <v>0</v>
+      </c>
+      <c r="Z295">
+        <v>0</v>
+      </c>
+      <c r="AA295">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A296">
+        <v>294</v>
+      </c>
+      <c r="B296">
+        <v>0</v>
+      </c>
+      <c r="C296" t="s">
+        <v>2</v>
+      </c>
+      <c r="D296" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E296">
+        <v>1</v>
+      </c>
+      <c r="H296">
+        <v>1271892280</v>
+      </c>
+      <c r="I296">
+        <v>4</v>
+      </c>
+      <c r="J296" t="s">
+        <v>128</v>
+      </c>
+      <c r="K296" t="s">
+        <v>1028</v>
+      </c>
+      <c r="L296" t="s">
+        <v>1030</v>
+      </c>
+      <c r="N296" s="14" t="s">
+        <v>676</v>
+      </c>
+      <c r="Q296">
+        <v>1</v>
+      </c>
+      <c r="R296">
+        <v>38</v>
+      </c>
+      <c r="S296">
+        <v>3</v>
+      </c>
+      <c r="T296" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="W296">
+        <v>1</v>
+      </c>
+      <c r="X296">
+        <v>0</v>
+      </c>
+      <c r="Y296">
+        <v>0</v>
+      </c>
+      <c r="Z296">
+        <v>0</v>
+      </c>
+      <c r="AA296">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A297">
+        <v>295</v>
+      </c>
+      <c r="B297">
+        <v>0</v>
+      </c>
+      <c r="C297" t="s">
+        <v>2</v>
+      </c>
+      <c r="D297" t="s">
+        <v>1030</v>
+      </c>
+      <c r="E297">
+        <v>1</v>
+      </c>
+      <c r="H297">
+        <v>1398307276</v>
+      </c>
+      <c r="I297">
+        <v>5</v>
+      </c>
+      <c r="J297" t="s">
+        <v>128</v>
+      </c>
+      <c r="K297" t="s">
+        <v>1029</v>
+      </c>
+      <c r="L297" t="s">
+        <v>1031</v>
+      </c>
+      <c r="N297" s="14" t="s">
+        <v>1032</v>
+      </c>
+      <c r="Q297">
+        <v>1</v>
+      </c>
+      <c r="R297">
+        <v>26</v>
+      </c>
+      <c r="S297">
+        <v>57</v>
+      </c>
+      <c r="T297" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="W297">
+        <v>1</v>
+      </c>
+      <c r="X297">
+        <v>0</v>
+      </c>
+      <c r="Y297">
+        <v>0</v>
+      </c>
+      <c r="Z297">
+        <v>0</v>
+      </c>
+      <c r="AA297">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A298">
+        <v>296</v>
+      </c>
+      <c r="B298">
+        <v>0</v>
+      </c>
+      <c r="C298" t="s">
+        <v>2</v>
+      </c>
+      <c r="D298" t="s">
+        <v>1031</v>
+      </c>
+      <c r="E298">
+        <v>1</v>
+      </c>
+      <c r="H298">
+        <v>2104681081</v>
+      </c>
+      <c r="I298">
+        <v>6</v>
+      </c>
+      <c r="J298" t="s">
+        <v>128</v>
+      </c>
+      <c r="K298" t="s">
+        <v>1030</v>
+      </c>
+      <c r="N298" s="14" t="s">
+        <v>955</v>
+      </c>
+      <c r="Q298">
+        <v>1</v>
+      </c>
+      <c r="R298">
+        <v>45</v>
+      </c>
+      <c r="S298">
+        <v>28</v>
+      </c>
+      <c r="T298" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="W298">
+        <v>1</v>
+      </c>
+      <c r="X298">
+        <v>0</v>
+      </c>
+      <c r="Y298">
+        <v>0</v>
+      </c>
+      <c r="Z298">
+        <v>0</v>
+      </c>
+      <c r="AA298">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A299">
+        <v>297</v>
+      </c>
+      <c r="B299">
+        <v>0</v>
+      </c>
+      <c r="C299" t="s">
+        <v>4</v>
+      </c>
+      <c r="D299" t="s">
+        <v>1033</v>
+      </c>
+      <c r="E299">
+        <v>12</v>
+      </c>
+      <c r="H299">
+        <v>3658044556</v>
+      </c>
+      <c r="I299">
+        <v>1</v>
+      </c>
+      <c r="J299" t="s">
+        <v>1033</v>
+      </c>
+      <c r="N299" s="14" t="s">
+        <v>1034</v>
+      </c>
+      <c r="O299" t="s">
+        <v>130</v>
+      </c>
+      <c r="P299">
+        <v>2015</v>
+      </c>
+      <c r="Q299">
+        <v>4</v>
+      </c>
+      <c r="R299">
+        <v>43</v>
+      </c>
+      <c r="S299">
+        <v>0</v>
+      </c>
+      <c r="T299" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="V299" t="s">
+        <v>163</v>
+      </c>
+      <c r="W299">
+        <v>1</v>
+      </c>
+      <c r="X299">
+        <v>0</v>
+      </c>
+      <c r="Y299">
+        <v>0</v>
+      </c>
+      <c r="Z299">
+        <v>0</v>
+      </c>
+      <c r="AA299">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A300">
+        <v>298</v>
+      </c>
+      <c r="B300">
+        <v>0</v>
+      </c>
+      <c r="C300" t="s">
+        <v>4</v>
+      </c>
+      <c r="D300" t="s">
+        <v>1035</v>
+      </c>
+      <c r="E300">
+        <v>12</v>
+      </c>
+      <c r="H300">
+        <v>5484348757</v>
+      </c>
+      <c r="I300">
+        <v>1</v>
+      </c>
+      <c r="J300" t="s">
+        <v>1035</v>
+      </c>
+      <c r="N300" s="14" t="s">
+        <v>1036</v>
+      </c>
+      <c r="O300" t="s">
+        <v>131</v>
+      </c>
+      <c r="P300">
+        <v>2016</v>
+      </c>
+      <c r="Q300">
+        <v>4</v>
+      </c>
+      <c r="R300">
+        <v>44</v>
+      </c>
+      <c r="S300">
+        <v>55</v>
+      </c>
+      <c r="T300" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="V300" t="s">
+        <v>163</v>
+      </c>
+      <c r="W300">
+        <v>1</v>
+      </c>
+      <c r="X300">
+        <v>0</v>
+      </c>
+      <c r="Y300">
+        <v>0</v>
+      </c>
+      <c r="Z300">
+        <v>0</v>
+      </c>
+      <c r="AA300">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A301">
+        <v>299</v>
+      </c>
+      <c r="B301">
+        <v>0</v>
+      </c>
+      <c r="C301" t="s">
+        <v>4</v>
+      </c>
+      <c r="D301" t="s">
+        <v>1039</v>
+      </c>
+      <c r="E301">
+        <v>24</v>
+      </c>
+      <c r="H301">
+        <v>2697805828</v>
+      </c>
+      <c r="I301">
+        <v>2</v>
+      </c>
+      <c r="J301" t="s">
+        <v>393</v>
+      </c>
+      <c r="K301" t="s">
+        <v>393</v>
+      </c>
+      <c r="N301" s="14" t="s">
+        <v>1040</v>
+      </c>
+      <c r="Q301">
+        <v>9</v>
+      </c>
+      <c r="R301">
+        <v>28</v>
+      </c>
+      <c r="S301">
+        <v>3</v>
+      </c>
+      <c r="V301" t="s">
+        <v>532</v>
+      </c>
+      <c r="W301">
+        <v>1</v>
+      </c>
+      <c r="X301">
+        <v>0</v>
+      </c>
+      <c r="Y301">
+        <v>0</v>
+      </c>
+      <c r="Z301">
+        <v>0</v>
+      </c>
+      <c r="AA301">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A302">
+        <v>300</v>
+      </c>
+      <c r="B302">
+        <v>0</v>
+      </c>
+      <c r="C302" t="s">
+        <v>4</v>
+      </c>
+      <c r="D302" t="s">
+        <v>1042</v>
+      </c>
+      <c r="E302">
+        <v>12</v>
+      </c>
+      <c r="H302">
+        <v>4135601130</v>
+      </c>
+      <c r="I302">
+        <v>1</v>
+      </c>
+      <c r="J302" t="s">
+        <v>1042</v>
+      </c>
+      <c r="N302" s="14" t="s">
+        <v>1043</v>
+      </c>
+      <c r="Q302">
+        <v>4</v>
+      </c>
+      <c r="R302">
+        <v>49</v>
+      </c>
+      <c r="S302">
+        <v>37</v>
+      </c>
+      <c r="T302" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="V302" t="s">
+        <v>163</v>
+      </c>
+      <c r="W302">
+        <v>1</v>
+      </c>
+      <c r="X302">
+        <v>0</v>
+      </c>
+      <c r="Y302">
+        <v>0</v>
+      </c>
+      <c r="Z302">
+        <v>0</v>
+      </c>
+      <c r="AA302">
         <v>0</v>
       </c>
     </row>
@@ -27700,8 +29205,8 @@
   </sheetPr>
   <dimension ref="A1:AG133"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+    <sheetView topLeftCell="E34" workbookViewId="0">
+      <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
DATABASE: fixed wrong entry, exported the updated version of the database
</commit_message>
<xml_diff>
--- a/resources/database/data/anime/db_anime - staging data.xlsx
+++ b/resources/database/data/anime/db_anime - staging data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="9000" windowWidth="24000" windowHeight="9495" tabRatio="856"/>
+    <workbookView xWindow="0" yWindow="9600" windowWidth="24000" windowHeight="9495" tabRatio="856"/>
   </bookViews>
   <sheets>
     <sheet name="&gt;&gt;Final" sheetId="1" r:id="rId1"/>
@@ -3651,9 +3651,9 @@
   <dimension ref="A1:AA302"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A275" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A268" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="D283" sqref="D283"/>
+      <selection pane="bottomLeft" activeCell="D278" sqref="D278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22010,6 +22010,9 @@
       </c>
       <c r="E282">
         <v>22</v>
+      </c>
+      <c r="F282">
+        <v>1</v>
       </c>
       <c r="H282">
         <v>6539796249</v>

</xml_diff>

<commit_message>
DATABASE: updated 1 entry, exported the updated version of the database
</commit_message>
<xml_diff>
--- a/resources/database/data/anime/db_anime - staging data.xlsx
+++ b/resources/database/data/anime/db_anime - staging data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="9600" windowWidth="24000" windowHeight="9495" tabRatio="856"/>
+    <workbookView xWindow="0" yWindow="10200" windowWidth="24000" windowHeight="9495" tabRatio="856"/>
   </bookViews>
   <sheets>
     <sheet name="&gt;&gt;Final" sheetId="1" r:id="rId1"/>
@@ -3650,10 +3650,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA302"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A268" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="D278" sqref="D278"/>
+      <selection pane="bottomLeft" activeCell="W135" sqref="A135:XFD135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12542,13 +12542,13 @@
         <v>24</v>
       </c>
       <c r="F135">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G135">
         <v>0</v>
       </c>
       <c r="H135">
-        <v>36589079279</v>
+        <v>37380147527</v>
       </c>
       <c r="I135">
         <v>1</v>
@@ -12569,13 +12569,13 @@
         <v>2015</v>
       </c>
       <c r="Q135">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="R135">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="S135">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="T135" s="1" t="s">
         <v>135</v>

</xml_diff>

<commit_message>
DATABASE: added a line of new data, exported the updated version of the database
</commit_message>
<xml_diff>
--- a/resources/database/data/anime/db_anime - staging data.xlsx
+++ b/resources/database/data/anime/db_anime - staging data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="10200" windowWidth="24000" windowHeight="9495" tabRatio="856"/>
+    <workbookView xWindow="0" yWindow="11400" windowWidth="24000" windowHeight="9495" tabRatio="856"/>
   </bookViews>
   <sheets>
     <sheet name="&gt;&gt;Final" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4951" uniqueCount="1044">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4959" uniqueCount="1046">
   <si>
     <t>Summer</t>
   </si>
@@ -3167,6 +3167,12 @@
   </si>
   <si>
     <t>2017-09-03</t>
+  </si>
+  <si>
+    <t>selector spread WIXOSS</t>
+  </si>
+  <si>
+    <t>2017-11-14</t>
   </si>
 </sst>
 </file>
@@ -3648,12 +3654,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA302"/>
+  <dimension ref="A1:AA303"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="W135" sqref="A135:XFD135"/>
+      <selection pane="bottomLeft" activeCell="N169" sqref="N169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14818,6 +14824,9 @@
       <c r="J169" t="s">
         <v>462</v>
       </c>
+      <c r="L169" t="s">
+        <v>1044</v>
+      </c>
       <c r="N169" s="14" t="s">
         <v>575</v>
       </c>
@@ -23294,6 +23303,71 @@
         <v>0</v>
       </c>
       <c r="AA302">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A303">
+        <v>301</v>
+      </c>
+      <c r="B303">
+        <v>0</v>
+      </c>
+      <c r="C303" t="s">
+        <v>2</v>
+      </c>
+      <c r="D303" t="s">
+        <v>1044</v>
+      </c>
+      <c r="E303">
+        <v>12</v>
+      </c>
+      <c r="H303">
+        <v>15163055693</v>
+      </c>
+      <c r="I303">
+        <v>2</v>
+      </c>
+      <c r="J303" t="s">
+        <v>462</v>
+      </c>
+      <c r="K303" t="s">
+        <v>462</v>
+      </c>
+      <c r="N303" s="14" t="s">
+        <v>1045</v>
+      </c>
+      <c r="O303" t="s">
+        <v>130</v>
+      </c>
+      <c r="P303">
+        <v>2013</v>
+      </c>
+      <c r="Q303">
+        <v>4</v>
+      </c>
+      <c r="R303">
+        <v>44</v>
+      </c>
+      <c r="S303">
+        <v>16</v>
+      </c>
+      <c r="T303" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="W303">
+        <v>1</v>
+      </c>
+      <c r="X303">
+        <v>0</v>
+      </c>
+      <c r="Y303">
+        <v>0</v>
+      </c>
+      <c r="Z303">
+        <v>0</v>
+      </c>
+      <c r="AA303">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DATABASE: added 1 line of new data to staging data, exported the updated version of the database
</commit_message>
<xml_diff>
--- a/resources/database/data/anime/db_anime - staging data.xlsx
+++ b/resources/database/data/anime/db_anime - staging data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="11400" windowWidth="24000" windowHeight="9495" tabRatio="856"/>
+    <workbookView xWindow="0" yWindow="12000" windowWidth="24000" windowHeight="9495" tabRatio="856"/>
   </bookViews>
   <sheets>
     <sheet name="&gt;&gt;Final" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4959" uniqueCount="1046">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4964" uniqueCount="1048">
   <si>
     <t>Summer</t>
   </si>
@@ -3173,6 +3173,12 @@
   </si>
   <si>
     <t>2017-11-14</t>
+  </si>
+  <si>
+    <t>Durarara!!</t>
+  </si>
+  <si>
+    <t>2017-11-25</t>
   </si>
 </sst>
 </file>
@@ -3654,12 +3660,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA303"/>
+  <dimension ref="A1:AA304"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A293" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="N169" sqref="N169"/>
+      <selection pane="bottomLeft" activeCell="H299" sqref="A3:AA304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23368,6 +23374,65 @@
         <v>0</v>
       </c>
       <c r="AA303">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="304" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A304">
+        <v>301</v>
+      </c>
+      <c r="B304">
+        <v>0</v>
+      </c>
+      <c r="C304" t="s">
+        <v>2</v>
+      </c>
+      <c r="D304" t="s">
+        <v>1046</v>
+      </c>
+      <c r="E304">
+        <v>25</v>
+      </c>
+      <c r="F304">
+        <v>1</v>
+      </c>
+      <c r="H304">
+        <v>27524967285</v>
+      </c>
+      <c r="I304">
+        <v>1</v>
+      </c>
+      <c r="J304" t="s">
+        <v>1046</v>
+      </c>
+      <c r="N304" s="14" t="s">
+        <v>1047</v>
+      </c>
+      <c r="Q304">
+        <v>10</v>
+      </c>
+      <c r="R304">
+        <v>34</v>
+      </c>
+      <c r="S304">
+        <v>22</v>
+      </c>
+      <c r="T304" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="W304">
+        <v>1</v>
+      </c>
+      <c r="X304">
+        <v>0</v>
+      </c>
+      <c r="Y304">
+        <v>0</v>
+      </c>
+      <c r="Z304">
+        <v>0</v>
+      </c>
+      <c r="AA304">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DATABASE: corrected one invalid line, added 4 lines of new data
</commit_message>
<xml_diff>
--- a/resources/database/data/anime/db_anime - staging data.xlsx
+++ b/resources/database/data/anime/db_anime - staging data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="12000" windowWidth="24000" windowHeight="9495" tabRatio="856"/>
+    <workbookView xWindow="0" yWindow="12600" windowWidth="24000" windowHeight="9495" tabRatio="856"/>
   </bookViews>
   <sheets>
     <sheet name="&gt;&gt;Final" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4964" uniqueCount="1048">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4989" uniqueCount="1056">
   <si>
     <t>Summer</t>
   </si>
@@ -3179,6 +3179,30 @@
   </si>
   <si>
     <t>2017-11-25</t>
+  </si>
+  <si>
+    <t>Bungou Stray Dogs</t>
+  </si>
+  <si>
+    <t>2017-12-06</t>
+  </si>
+  <si>
+    <t>Kuroko no Basket</t>
+  </si>
+  <si>
+    <t>Kuroko no Basket S2</t>
+  </si>
+  <si>
+    <t>Kuroko no Basket S3</t>
+  </si>
+  <si>
+    <t>2017-12-08</t>
+  </si>
+  <si>
+    <t>2017-12-12</t>
+  </si>
+  <si>
+    <t>2017-12-14</t>
   </si>
 </sst>
 </file>
@@ -3660,12 +3684,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA304"/>
+  <dimension ref="A1:AA308"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A293" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="H299" sqref="A3:AA304"/>
+      <selection pane="bottomLeft" activeCell="A302" sqref="A302:B308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23379,7 +23403,7 @@
     </row>
     <row r="304" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A304">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B304">
         <v>0</v>
@@ -23433,6 +23457,248 @@
         <v>0</v>
       </c>
       <c r="AA304">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="305" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A305">
+        <v>303</v>
+      </c>
+      <c r="B305">
+        <v>0</v>
+      </c>
+      <c r="C305" t="s">
+        <v>4</v>
+      </c>
+      <c r="D305" t="s">
+        <v>1048</v>
+      </c>
+      <c r="E305">
+        <v>24</v>
+      </c>
+      <c r="H305">
+        <v>8113709673</v>
+      </c>
+      <c r="I305">
+        <v>1</v>
+      </c>
+      <c r="J305" t="s">
+        <v>1048</v>
+      </c>
+      <c r="N305" s="14" t="s">
+        <v>1049</v>
+      </c>
+      <c r="O305" t="s">
+        <v>131</v>
+      </c>
+      <c r="P305">
+        <v>2016</v>
+      </c>
+      <c r="Q305">
+        <v>9</v>
+      </c>
+      <c r="R305">
+        <v>28</v>
+      </c>
+      <c r="S305">
+        <v>3</v>
+      </c>
+      <c r="T305" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="W305">
+        <v>1</v>
+      </c>
+      <c r="X305">
+        <v>0</v>
+      </c>
+      <c r="Y305">
+        <v>0</v>
+      </c>
+      <c r="Z305">
+        <v>0</v>
+      </c>
+      <c r="AA305">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="306" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A306">
+        <v>304</v>
+      </c>
+      <c r="B306">
+        <v>0</v>
+      </c>
+      <c r="C306" t="s">
+        <v>4</v>
+      </c>
+      <c r="D306" t="s">
+        <v>1050</v>
+      </c>
+      <c r="E306">
+        <v>25</v>
+      </c>
+      <c r="H306">
+        <v>6528361435</v>
+      </c>
+      <c r="I306">
+        <v>1</v>
+      </c>
+      <c r="J306" t="s">
+        <v>1050</v>
+      </c>
+      <c r="L306" t="s">
+        <v>1051</v>
+      </c>
+      <c r="N306" s="14" t="s">
+        <v>1053</v>
+      </c>
+      <c r="Q306">
+        <v>10</v>
+      </c>
+      <c r="R306">
+        <v>5</v>
+      </c>
+      <c r="S306">
+        <v>59</v>
+      </c>
+      <c r="V306" t="s">
+        <v>1011</v>
+      </c>
+      <c r="W306">
+        <v>1</v>
+      </c>
+      <c r="X306">
+        <v>0</v>
+      </c>
+      <c r="Y306">
+        <v>0</v>
+      </c>
+      <c r="Z306">
+        <v>0</v>
+      </c>
+      <c r="AA306">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="307" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A307">
+        <v>305</v>
+      </c>
+      <c r="B307">
+        <v>0</v>
+      </c>
+      <c r="C307" t="s">
+        <v>4</v>
+      </c>
+      <c r="D307" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E307">
+        <v>25</v>
+      </c>
+      <c r="H307">
+        <v>6826328734</v>
+      </c>
+      <c r="I307">
+        <v>2</v>
+      </c>
+      <c r="J307" t="s">
+        <v>1050</v>
+      </c>
+      <c r="K307" t="s">
+        <v>1050</v>
+      </c>
+      <c r="L307" t="s">
+        <v>1052</v>
+      </c>
+      <c r="N307" s="14" t="s">
+        <v>1054</v>
+      </c>
+      <c r="Q307">
+        <v>10</v>
+      </c>
+      <c r="R307">
+        <v>6</v>
+      </c>
+      <c r="S307">
+        <v>10</v>
+      </c>
+      <c r="V307" t="s">
+        <v>1011</v>
+      </c>
+      <c r="W307">
+        <v>1</v>
+      </c>
+      <c r="X307">
+        <v>0</v>
+      </c>
+      <c r="Y307">
+        <v>0</v>
+      </c>
+      <c r="Z307">
+        <v>0</v>
+      </c>
+      <c r="AA307">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="308" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A308">
+        <v>306</v>
+      </c>
+      <c r="B308">
+        <v>0</v>
+      </c>
+      <c r="C308" t="s">
+        <v>4</v>
+      </c>
+      <c r="D308" t="s">
+        <v>1052</v>
+      </c>
+      <c r="E308">
+        <v>25</v>
+      </c>
+      <c r="H308">
+        <v>6725836945</v>
+      </c>
+      <c r="I308">
+        <v>3</v>
+      </c>
+      <c r="J308" t="s">
+        <v>1050</v>
+      </c>
+      <c r="K308" t="s">
+        <v>1051</v>
+      </c>
+      <c r="N308" s="14" t="s">
+        <v>1055</v>
+      </c>
+      <c r="Q308">
+        <v>10</v>
+      </c>
+      <c r="R308">
+        <v>6</v>
+      </c>
+      <c r="S308">
+        <v>35</v>
+      </c>
+      <c r="V308" t="s">
+        <v>1011</v>
+      </c>
+      <c r="W308">
+        <v>1</v>
+      </c>
+      <c r="X308">
+        <v>0</v>
+      </c>
+      <c r="Y308">
+        <v>0</v>
+      </c>
+      <c r="Z308">
+        <v>0</v>
+      </c>
+      <c r="AA308">
         <v>0</v>
       </c>
     </row>

</xml_diff>